<commit_message>
EDI filt chla updates
</commit_message>
<xml_diff>
--- a/Data/DataAlreadyUploadedToEDI/EDIProductionFiles/MakeEMLFilteredChlorophyll/data/2022_data/chl_calculations/Sunapee Chl run 7Mar23.xlsx
+++ b/Data/DataAlreadyUploadedToEDI/EDIProductionFiles/MakeEMLFilteredChlorophyll/data/2022_data/chl_calculations/Sunapee Chl run 7Mar23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwoel\Dropbox\Thesis\Data\analytical chemistry\chla_extraction\chla calculations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abreefpilz\Documents\GitHub\Reservoirs\Data\DataAlreadyUploadedToEDI\EDIProductionFiles\MakeEMLFilteredChlorophyll\data\2022_data\chl_calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4EF97E-F394-42A8-BEE3-C9ACD6B874CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268FB66E-C048-43D0-ABC5-81002E20ABB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calculations" sheetId="2" r:id="rId1"/>
@@ -353,40 +353,40 @@
     <t>blank 15</t>
   </si>
   <si>
-    <t>F50 03Feb23 1.6m</t>
+    <t>F50_03Feb2023_1.6_DUP</t>
   </si>
   <si>
-    <t>SUNP 29Jun22 1.0</t>
+    <t>S50_29Jun2022_1.0</t>
   </si>
   <si>
-    <t>SUNP 16Jun22 1.0</t>
+    <t>S50_16Jun2022_1.0</t>
   </si>
   <si>
-    <t>SUNP 19Jul22 1.0</t>
+    <t>S50_19Jul2022_1.0</t>
   </si>
   <si>
-    <t>SUNP 07Jul22 8.0</t>
+    <t>S50_07Jul2022_8.0</t>
   </si>
   <si>
-    <t>SUNP 16Jun22 8.0</t>
+    <t>S50_29Jun2022_8.0</t>
   </si>
   <si>
-    <t>SUNP 29Jun22 8.0</t>
+    <t>S50_16Jun2022_8.0</t>
   </si>
   <si>
-    <t>SUNP 19Jul22 8.0</t>
+    <t>S50_19Jul2022_8.0</t>
   </si>
   <si>
-    <t>SUNP 13Jul22 1.0</t>
+    <t>S50_13Jul2022_1.0</t>
   </si>
   <si>
-    <t>SUNP 13Jul22 8.0</t>
+    <t>S50_13Jul2022_8.0</t>
   </si>
   <si>
-    <t>SUNP 26Jul22 8.0</t>
+    <t>S50_26Jul2022_8.0</t>
   </si>
   <si>
-    <t>SUNP 26Jul22 1.0</t>
+    <t>S50_26Jul2022_1.0</t>
   </si>
 </sst>
 </file>
@@ -5340,341 +5340,341 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="27" style="3" customWidth="1"/>
     <col min="2" max="2" width="12" style="3" customWidth="1"/>
-    <col min="3" max="15" width="10.7265625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="22.453125" style="3" customWidth="1"/>
-    <col min="17" max="18" width="23.6328125" style="3" customWidth="1"/>
-    <col min="19" max="35" width="10.7265625" style="3" customWidth="1"/>
-    <col min="36" max="37" width="10.7265625" style="4" customWidth="1"/>
-    <col min="38" max="39" width="10.7265625" style="3" customWidth="1"/>
-    <col min="40" max="49" width="8.7265625" style="3"/>
-    <col min="50" max="50" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="51" max="252" width="8.7265625" style="3"/>
-    <col min="253" max="254" width="18.54296875" style="3" customWidth="1"/>
-    <col min="255" max="270" width="8.7265625" style="3"/>
-    <col min="271" max="271" width="13.81640625" style="3" customWidth="1"/>
-    <col min="272" max="272" width="16.81640625" style="3" customWidth="1"/>
-    <col min="273" max="508" width="8.7265625" style="3"/>
-    <col min="509" max="510" width="18.54296875" style="3" customWidth="1"/>
-    <col min="511" max="526" width="8.7265625" style="3"/>
-    <col min="527" max="527" width="13.81640625" style="3" customWidth="1"/>
-    <col min="528" max="528" width="16.81640625" style="3" customWidth="1"/>
-    <col min="529" max="764" width="8.7265625" style="3"/>
-    <col min="765" max="766" width="18.54296875" style="3" customWidth="1"/>
-    <col min="767" max="782" width="8.7265625" style="3"/>
-    <col min="783" max="783" width="13.81640625" style="3" customWidth="1"/>
-    <col min="784" max="784" width="16.81640625" style="3" customWidth="1"/>
-    <col min="785" max="1020" width="8.7265625" style="3"/>
-    <col min="1021" max="1022" width="18.54296875" style="3" customWidth="1"/>
-    <col min="1023" max="1038" width="8.7265625" style="3"/>
-    <col min="1039" max="1039" width="13.81640625" style="3" customWidth="1"/>
-    <col min="1040" max="1040" width="16.81640625" style="3" customWidth="1"/>
-    <col min="1041" max="1276" width="8.7265625" style="3"/>
-    <col min="1277" max="1278" width="18.54296875" style="3" customWidth="1"/>
-    <col min="1279" max="1294" width="8.7265625" style="3"/>
-    <col min="1295" max="1295" width="13.81640625" style="3" customWidth="1"/>
-    <col min="1296" max="1296" width="16.81640625" style="3" customWidth="1"/>
-    <col min="1297" max="1532" width="8.7265625" style="3"/>
-    <col min="1533" max="1534" width="18.54296875" style="3" customWidth="1"/>
-    <col min="1535" max="1550" width="8.7265625" style="3"/>
-    <col min="1551" max="1551" width="13.81640625" style="3" customWidth="1"/>
-    <col min="1552" max="1552" width="16.81640625" style="3" customWidth="1"/>
-    <col min="1553" max="1788" width="8.7265625" style="3"/>
-    <col min="1789" max="1790" width="18.54296875" style="3" customWidth="1"/>
-    <col min="1791" max="1806" width="8.7265625" style="3"/>
-    <col min="1807" max="1807" width="13.81640625" style="3" customWidth="1"/>
-    <col min="1808" max="1808" width="16.81640625" style="3" customWidth="1"/>
-    <col min="1809" max="2044" width="8.7265625" style="3"/>
-    <col min="2045" max="2046" width="18.54296875" style="3" customWidth="1"/>
-    <col min="2047" max="2062" width="8.7265625" style="3"/>
-    <col min="2063" max="2063" width="13.81640625" style="3" customWidth="1"/>
-    <col min="2064" max="2064" width="16.81640625" style="3" customWidth="1"/>
-    <col min="2065" max="2300" width="8.7265625" style="3"/>
-    <col min="2301" max="2302" width="18.54296875" style="3" customWidth="1"/>
-    <col min="2303" max="2318" width="8.7265625" style="3"/>
-    <col min="2319" max="2319" width="13.81640625" style="3" customWidth="1"/>
-    <col min="2320" max="2320" width="16.81640625" style="3" customWidth="1"/>
-    <col min="2321" max="2556" width="8.7265625" style="3"/>
-    <col min="2557" max="2558" width="18.54296875" style="3" customWidth="1"/>
-    <col min="2559" max="2574" width="8.7265625" style="3"/>
-    <col min="2575" max="2575" width="13.81640625" style="3" customWidth="1"/>
-    <col min="2576" max="2576" width="16.81640625" style="3" customWidth="1"/>
-    <col min="2577" max="2812" width="8.7265625" style="3"/>
-    <col min="2813" max="2814" width="18.54296875" style="3" customWidth="1"/>
-    <col min="2815" max="2830" width="8.7265625" style="3"/>
-    <col min="2831" max="2831" width="13.81640625" style="3" customWidth="1"/>
-    <col min="2832" max="2832" width="16.81640625" style="3" customWidth="1"/>
-    <col min="2833" max="3068" width="8.7265625" style="3"/>
-    <col min="3069" max="3070" width="18.54296875" style="3" customWidth="1"/>
-    <col min="3071" max="3086" width="8.7265625" style="3"/>
-    <col min="3087" max="3087" width="13.81640625" style="3" customWidth="1"/>
-    <col min="3088" max="3088" width="16.81640625" style="3" customWidth="1"/>
-    <col min="3089" max="3324" width="8.7265625" style="3"/>
-    <col min="3325" max="3326" width="18.54296875" style="3" customWidth="1"/>
-    <col min="3327" max="3342" width="8.7265625" style="3"/>
-    <col min="3343" max="3343" width="13.81640625" style="3" customWidth="1"/>
-    <col min="3344" max="3344" width="16.81640625" style="3" customWidth="1"/>
-    <col min="3345" max="3580" width="8.7265625" style="3"/>
-    <col min="3581" max="3582" width="18.54296875" style="3" customWidth="1"/>
-    <col min="3583" max="3598" width="8.7265625" style="3"/>
-    <col min="3599" max="3599" width="13.81640625" style="3" customWidth="1"/>
-    <col min="3600" max="3600" width="16.81640625" style="3" customWidth="1"/>
-    <col min="3601" max="3836" width="8.7265625" style="3"/>
-    <col min="3837" max="3838" width="18.54296875" style="3" customWidth="1"/>
-    <col min="3839" max="3854" width="8.7265625" style="3"/>
-    <col min="3855" max="3855" width="13.81640625" style="3" customWidth="1"/>
-    <col min="3856" max="3856" width="16.81640625" style="3" customWidth="1"/>
-    <col min="3857" max="4092" width="8.7265625" style="3"/>
-    <col min="4093" max="4094" width="18.54296875" style="3" customWidth="1"/>
-    <col min="4095" max="4110" width="8.7265625" style="3"/>
-    <col min="4111" max="4111" width="13.81640625" style="3" customWidth="1"/>
-    <col min="4112" max="4112" width="16.81640625" style="3" customWidth="1"/>
-    <col min="4113" max="4348" width="8.7265625" style="3"/>
-    <col min="4349" max="4350" width="18.54296875" style="3" customWidth="1"/>
-    <col min="4351" max="4366" width="8.7265625" style="3"/>
-    <col min="4367" max="4367" width="13.81640625" style="3" customWidth="1"/>
-    <col min="4368" max="4368" width="16.81640625" style="3" customWidth="1"/>
-    <col min="4369" max="4604" width="8.7265625" style="3"/>
-    <col min="4605" max="4606" width="18.54296875" style="3" customWidth="1"/>
-    <col min="4607" max="4622" width="8.7265625" style="3"/>
-    <col min="4623" max="4623" width="13.81640625" style="3" customWidth="1"/>
-    <col min="4624" max="4624" width="16.81640625" style="3" customWidth="1"/>
-    <col min="4625" max="4860" width="8.7265625" style="3"/>
-    <col min="4861" max="4862" width="18.54296875" style="3" customWidth="1"/>
-    <col min="4863" max="4878" width="8.7265625" style="3"/>
-    <col min="4879" max="4879" width="13.81640625" style="3" customWidth="1"/>
-    <col min="4880" max="4880" width="16.81640625" style="3" customWidth="1"/>
-    <col min="4881" max="5116" width="8.7265625" style="3"/>
-    <col min="5117" max="5118" width="18.54296875" style="3" customWidth="1"/>
-    <col min="5119" max="5134" width="8.7265625" style="3"/>
-    <col min="5135" max="5135" width="13.81640625" style="3" customWidth="1"/>
-    <col min="5136" max="5136" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5137" max="5372" width="8.7265625" style="3"/>
-    <col min="5373" max="5374" width="18.54296875" style="3" customWidth="1"/>
-    <col min="5375" max="5390" width="8.7265625" style="3"/>
-    <col min="5391" max="5391" width="13.81640625" style="3" customWidth="1"/>
-    <col min="5392" max="5392" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5393" max="5628" width="8.7265625" style="3"/>
-    <col min="5629" max="5630" width="18.54296875" style="3" customWidth="1"/>
-    <col min="5631" max="5646" width="8.7265625" style="3"/>
-    <col min="5647" max="5647" width="13.81640625" style="3" customWidth="1"/>
-    <col min="5648" max="5648" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5649" max="5884" width="8.7265625" style="3"/>
-    <col min="5885" max="5886" width="18.54296875" style="3" customWidth="1"/>
-    <col min="5887" max="5902" width="8.7265625" style="3"/>
-    <col min="5903" max="5903" width="13.81640625" style="3" customWidth="1"/>
-    <col min="5904" max="5904" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5905" max="6140" width="8.7265625" style="3"/>
-    <col min="6141" max="6142" width="18.54296875" style="3" customWidth="1"/>
-    <col min="6143" max="6158" width="8.7265625" style="3"/>
-    <col min="6159" max="6159" width="13.81640625" style="3" customWidth="1"/>
-    <col min="6160" max="6160" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6161" max="6396" width="8.7265625" style="3"/>
-    <col min="6397" max="6398" width="18.54296875" style="3" customWidth="1"/>
-    <col min="6399" max="6414" width="8.7265625" style="3"/>
-    <col min="6415" max="6415" width="13.81640625" style="3" customWidth="1"/>
-    <col min="6416" max="6416" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6417" max="6652" width="8.7265625" style="3"/>
-    <col min="6653" max="6654" width="18.54296875" style="3" customWidth="1"/>
-    <col min="6655" max="6670" width="8.7265625" style="3"/>
-    <col min="6671" max="6671" width="13.81640625" style="3" customWidth="1"/>
-    <col min="6672" max="6672" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6673" max="6908" width="8.7265625" style="3"/>
-    <col min="6909" max="6910" width="18.54296875" style="3" customWidth="1"/>
-    <col min="6911" max="6926" width="8.7265625" style="3"/>
-    <col min="6927" max="6927" width="13.81640625" style="3" customWidth="1"/>
-    <col min="6928" max="6928" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6929" max="7164" width="8.7265625" style="3"/>
-    <col min="7165" max="7166" width="18.54296875" style="3" customWidth="1"/>
-    <col min="7167" max="7182" width="8.7265625" style="3"/>
-    <col min="7183" max="7183" width="13.81640625" style="3" customWidth="1"/>
-    <col min="7184" max="7184" width="16.81640625" style="3" customWidth="1"/>
-    <col min="7185" max="7420" width="8.7265625" style="3"/>
-    <col min="7421" max="7422" width="18.54296875" style="3" customWidth="1"/>
-    <col min="7423" max="7438" width="8.7265625" style="3"/>
-    <col min="7439" max="7439" width="13.81640625" style="3" customWidth="1"/>
-    <col min="7440" max="7440" width="16.81640625" style="3" customWidth="1"/>
-    <col min="7441" max="7676" width="8.7265625" style="3"/>
-    <col min="7677" max="7678" width="18.54296875" style="3" customWidth="1"/>
-    <col min="7679" max="7694" width="8.7265625" style="3"/>
-    <col min="7695" max="7695" width="13.81640625" style="3" customWidth="1"/>
-    <col min="7696" max="7696" width="16.81640625" style="3" customWidth="1"/>
-    <col min="7697" max="7932" width="8.7265625" style="3"/>
-    <col min="7933" max="7934" width="18.54296875" style="3" customWidth="1"/>
-    <col min="7935" max="7950" width="8.7265625" style="3"/>
-    <col min="7951" max="7951" width="13.81640625" style="3" customWidth="1"/>
-    <col min="7952" max="7952" width="16.81640625" style="3" customWidth="1"/>
-    <col min="7953" max="8188" width="8.7265625" style="3"/>
-    <col min="8189" max="8190" width="18.54296875" style="3" customWidth="1"/>
-    <col min="8191" max="8206" width="8.7265625" style="3"/>
-    <col min="8207" max="8207" width="13.81640625" style="3" customWidth="1"/>
-    <col min="8208" max="8208" width="16.81640625" style="3" customWidth="1"/>
-    <col min="8209" max="8444" width="8.7265625" style="3"/>
-    <col min="8445" max="8446" width="18.54296875" style="3" customWidth="1"/>
-    <col min="8447" max="8462" width="8.7265625" style="3"/>
-    <col min="8463" max="8463" width="13.81640625" style="3" customWidth="1"/>
-    <col min="8464" max="8464" width="16.81640625" style="3" customWidth="1"/>
-    <col min="8465" max="8700" width="8.7265625" style="3"/>
-    <col min="8701" max="8702" width="18.54296875" style="3" customWidth="1"/>
-    <col min="8703" max="8718" width="8.7265625" style="3"/>
-    <col min="8719" max="8719" width="13.81640625" style="3" customWidth="1"/>
-    <col min="8720" max="8720" width="16.81640625" style="3" customWidth="1"/>
-    <col min="8721" max="8956" width="8.7265625" style="3"/>
-    <col min="8957" max="8958" width="18.54296875" style="3" customWidth="1"/>
-    <col min="8959" max="8974" width="8.7265625" style="3"/>
-    <col min="8975" max="8975" width="13.81640625" style="3" customWidth="1"/>
-    <col min="8976" max="8976" width="16.81640625" style="3" customWidth="1"/>
-    <col min="8977" max="9212" width="8.7265625" style="3"/>
-    <col min="9213" max="9214" width="18.54296875" style="3" customWidth="1"/>
-    <col min="9215" max="9230" width="8.7265625" style="3"/>
-    <col min="9231" max="9231" width="13.81640625" style="3" customWidth="1"/>
-    <col min="9232" max="9232" width="16.81640625" style="3" customWidth="1"/>
-    <col min="9233" max="9468" width="8.7265625" style="3"/>
-    <col min="9469" max="9470" width="18.54296875" style="3" customWidth="1"/>
-    <col min="9471" max="9486" width="8.7265625" style="3"/>
-    <col min="9487" max="9487" width="13.81640625" style="3" customWidth="1"/>
-    <col min="9488" max="9488" width="16.81640625" style="3" customWidth="1"/>
-    <col min="9489" max="9724" width="8.7265625" style="3"/>
-    <col min="9725" max="9726" width="18.54296875" style="3" customWidth="1"/>
-    <col min="9727" max="9742" width="8.7265625" style="3"/>
-    <col min="9743" max="9743" width="13.81640625" style="3" customWidth="1"/>
-    <col min="9744" max="9744" width="16.81640625" style="3" customWidth="1"/>
-    <col min="9745" max="9980" width="8.7265625" style="3"/>
-    <col min="9981" max="9982" width="18.54296875" style="3" customWidth="1"/>
-    <col min="9983" max="9998" width="8.7265625" style="3"/>
-    <col min="9999" max="9999" width="13.81640625" style="3" customWidth="1"/>
-    <col min="10000" max="10000" width="16.81640625" style="3" customWidth="1"/>
-    <col min="10001" max="10236" width="8.7265625" style="3"/>
-    <col min="10237" max="10238" width="18.54296875" style="3" customWidth="1"/>
-    <col min="10239" max="10254" width="8.7265625" style="3"/>
-    <col min="10255" max="10255" width="13.81640625" style="3" customWidth="1"/>
-    <col min="10256" max="10256" width="16.81640625" style="3" customWidth="1"/>
-    <col min="10257" max="10492" width="8.7265625" style="3"/>
-    <col min="10493" max="10494" width="18.54296875" style="3" customWidth="1"/>
-    <col min="10495" max="10510" width="8.7265625" style="3"/>
-    <col min="10511" max="10511" width="13.81640625" style="3" customWidth="1"/>
-    <col min="10512" max="10512" width="16.81640625" style="3" customWidth="1"/>
-    <col min="10513" max="10748" width="8.7265625" style="3"/>
-    <col min="10749" max="10750" width="18.54296875" style="3" customWidth="1"/>
-    <col min="10751" max="10766" width="8.7265625" style="3"/>
-    <col min="10767" max="10767" width="13.81640625" style="3" customWidth="1"/>
-    <col min="10768" max="10768" width="16.81640625" style="3" customWidth="1"/>
-    <col min="10769" max="11004" width="8.7265625" style="3"/>
-    <col min="11005" max="11006" width="18.54296875" style="3" customWidth="1"/>
-    <col min="11007" max="11022" width="8.7265625" style="3"/>
-    <col min="11023" max="11023" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11024" max="11024" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11025" max="11260" width="8.7265625" style="3"/>
-    <col min="11261" max="11262" width="18.54296875" style="3" customWidth="1"/>
-    <col min="11263" max="11278" width="8.7265625" style="3"/>
-    <col min="11279" max="11279" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11280" max="11280" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11281" max="11516" width="8.7265625" style="3"/>
-    <col min="11517" max="11518" width="18.54296875" style="3" customWidth="1"/>
-    <col min="11519" max="11534" width="8.7265625" style="3"/>
-    <col min="11535" max="11535" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11536" max="11536" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11537" max="11772" width="8.7265625" style="3"/>
-    <col min="11773" max="11774" width="18.54296875" style="3" customWidth="1"/>
-    <col min="11775" max="11790" width="8.7265625" style="3"/>
-    <col min="11791" max="11791" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11792" max="11792" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11793" max="12028" width="8.7265625" style="3"/>
-    <col min="12029" max="12030" width="18.54296875" style="3" customWidth="1"/>
-    <col min="12031" max="12046" width="8.7265625" style="3"/>
-    <col min="12047" max="12047" width="13.81640625" style="3" customWidth="1"/>
-    <col min="12048" max="12048" width="16.81640625" style="3" customWidth="1"/>
-    <col min="12049" max="12284" width="8.7265625" style="3"/>
-    <col min="12285" max="12286" width="18.54296875" style="3" customWidth="1"/>
-    <col min="12287" max="12302" width="8.7265625" style="3"/>
-    <col min="12303" max="12303" width="13.81640625" style="3" customWidth="1"/>
-    <col min="12304" max="12304" width="16.81640625" style="3" customWidth="1"/>
-    <col min="12305" max="12540" width="8.7265625" style="3"/>
-    <col min="12541" max="12542" width="18.54296875" style="3" customWidth="1"/>
-    <col min="12543" max="12558" width="8.7265625" style="3"/>
-    <col min="12559" max="12559" width="13.81640625" style="3" customWidth="1"/>
-    <col min="12560" max="12560" width="16.81640625" style="3" customWidth="1"/>
-    <col min="12561" max="12796" width="8.7265625" style="3"/>
-    <col min="12797" max="12798" width="18.54296875" style="3" customWidth="1"/>
-    <col min="12799" max="12814" width="8.7265625" style="3"/>
-    <col min="12815" max="12815" width="13.81640625" style="3" customWidth="1"/>
-    <col min="12816" max="12816" width="16.81640625" style="3" customWidth="1"/>
-    <col min="12817" max="13052" width="8.7265625" style="3"/>
-    <col min="13053" max="13054" width="18.54296875" style="3" customWidth="1"/>
-    <col min="13055" max="13070" width="8.7265625" style="3"/>
-    <col min="13071" max="13071" width="13.81640625" style="3" customWidth="1"/>
-    <col min="13072" max="13072" width="16.81640625" style="3" customWidth="1"/>
-    <col min="13073" max="13308" width="8.7265625" style="3"/>
-    <col min="13309" max="13310" width="18.54296875" style="3" customWidth="1"/>
-    <col min="13311" max="13326" width="8.7265625" style="3"/>
-    <col min="13327" max="13327" width="13.81640625" style="3" customWidth="1"/>
-    <col min="13328" max="13328" width="16.81640625" style="3" customWidth="1"/>
-    <col min="13329" max="13564" width="8.7265625" style="3"/>
-    <col min="13565" max="13566" width="18.54296875" style="3" customWidth="1"/>
-    <col min="13567" max="13582" width="8.7265625" style="3"/>
-    <col min="13583" max="13583" width="13.81640625" style="3" customWidth="1"/>
-    <col min="13584" max="13584" width="16.81640625" style="3" customWidth="1"/>
-    <col min="13585" max="13820" width="8.7265625" style="3"/>
-    <col min="13821" max="13822" width="18.54296875" style="3" customWidth="1"/>
-    <col min="13823" max="13838" width="8.7265625" style="3"/>
-    <col min="13839" max="13839" width="13.81640625" style="3" customWidth="1"/>
-    <col min="13840" max="13840" width="16.81640625" style="3" customWidth="1"/>
-    <col min="13841" max="14076" width="8.7265625" style="3"/>
-    <col min="14077" max="14078" width="18.54296875" style="3" customWidth="1"/>
-    <col min="14079" max="14094" width="8.7265625" style="3"/>
-    <col min="14095" max="14095" width="13.81640625" style="3" customWidth="1"/>
-    <col min="14096" max="14096" width="16.81640625" style="3" customWidth="1"/>
-    <col min="14097" max="14332" width="8.7265625" style="3"/>
-    <col min="14333" max="14334" width="18.54296875" style="3" customWidth="1"/>
-    <col min="14335" max="14350" width="8.7265625" style="3"/>
-    <col min="14351" max="14351" width="13.81640625" style="3" customWidth="1"/>
-    <col min="14352" max="14352" width="16.81640625" style="3" customWidth="1"/>
-    <col min="14353" max="14588" width="8.7265625" style="3"/>
-    <col min="14589" max="14590" width="18.54296875" style="3" customWidth="1"/>
-    <col min="14591" max="14606" width="8.7265625" style="3"/>
-    <col min="14607" max="14607" width="13.81640625" style="3" customWidth="1"/>
-    <col min="14608" max="14608" width="16.81640625" style="3" customWidth="1"/>
-    <col min="14609" max="14844" width="8.7265625" style="3"/>
-    <col min="14845" max="14846" width="18.54296875" style="3" customWidth="1"/>
-    <col min="14847" max="14862" width="8.7265625" style="3"/>
-    <col min="14863" max="14863" width="13.81640625" style="3" customWidth="1"/>
-    <col min="14864" max="14864" width="16.81640625" style="3" customWidth="1"/>
-    <col min="14865" max="15100" width="8.7265625" style="3"/>
-    <col min="15101" max="15102" width="18.54296875" style="3" customWidth="1"/>
-    <col min="15103" max="15118" width="8.7265625" style="3"/>
-    <col min="15119" max="15119" width="13.81640625" style="3" customWidth="1"/>
-    <col min="15120" max="15120" width="16.81640625" style="3" customWidth="1"/>
-    <col min="15121" max="15356" width="8.7265625" style="3"/>
-    <col min="15357" max="15358" width="18.54296875" style="3" customWidth="1"/>
-    <col min="15359" max="15374" width="8.7265625" style="3"/>
-    <col min="15375" max="15375" width="13.81640625" style="3" customWidth="1"/>
-    <col min="15376" max="15376" width="16.81640625" style="3" customWidth="1"/>
-    <col min="15377" max="15612" width="8.7265625" style="3"/>
-    <col min="15613" max="15614" width="18.54296875" style="3" customWidth="1"/>
-    <col min="15615" max="15630" width="8.7265625" style="3"/>
-    <col min="15631" max="15631" width="13.81640625" style="3" customWidth="1"/>
-    <col min="15632" max="15632" width="16.81640625" style="3" customWidth="1"/>
-    <col min="15633" max="15868" width="8.7265625" style="3"/>
-    <col min="15869" max="15870" width="18.54296875" style="3" customWidth="1"/>
-    <col min="15871" max="15886" width="8.7265625" style="3"/>
-    <col min="15887" max="15887" width="13.81640625" style="3" customWidth="1"/>
-    <col min="15888" max="15888" width="16.81640625" style="3" customWidth="1"/>
-    <col min="15889" max="16124" width="8.7265625" style="3"/>
-    <col min="16125" max="16126" width="18.54296875" style="3" customWidth="1"/>
-    <col min="16127" max="16142" width="8.7265625" style="3"/>
-    <col min="16143" max="16143" width="13.81640625" style="3" customWidth="1"/>
-    <col min="16144" max="16144" width="16.81640625" style="3" customWidth="1"/>
-    <col min="16145" max="16384" width="8.7265625" style="3"/>
+    <col min="3" max="15" width="10.734375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="22.47265625" style="3" customWidth="1"/>
+    <col min="17" max="18" width="23.62890625" style="3" customWidth="1"/>
+    <col min="19" max="35" width="10.734375" style="3" customWidth="1"/>
+    <col min="36" max="37" width="10.734375" style="4" customWidth="1"/>
+    <col min="38" max="39" width="10.734375" style="3" customWidth="1"/>
+    <col min="40" max="49" width="8.734375" style="3"/>
+    <col min="50" max="50" width="12.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="252" width="8.734375" style="3"/>
+    <col min="253" max="254" width="18.5234375" style="3" customWidth="1"/>
+    <col min="255" max="270" width="8.734375" style="3"/>
+    <col min="271" max="271" width="13.7890625" style="3" customWidth="1"/>
+    <col min="272" max="272" width="16.7890625" style="3" customWidth="1"/>
+    <col min="273" max="508" width="8.734375" style="3"/>
+    <col min="509" max="510" width="18.5234375" style="3" customWidth="1"/>
+    <col min="511" max="526" width="8.734375" style="3"/>
+    <col min="527" max="527" width="13.7890625" style="3" customWidth="1"/>
+    <col min="528" max="528" width="16.7890625" style="3" customWidth="1"/>
+    <col min="529" max="764" width="8.734375" style="3"/>
+    <col min="765" max="766" width="18.5234375" style="3" customWidth="1"/>
+    <col min="767" max="782" width="8.734375" style="3"/>
+    <col min="783" max="783" width="13.7890625" style="3" customWidth="1"/>
+    <col min="784" max="784" width="16.7890625" style="3" customWidth="1"/>
+    <col min="785" max="1020" width="8.734375" style="3"/>
+    <col min="1021" max="1022" width="18.5234375" style="3" customWidth="1"/>
+    <col min="1023" max="1038" width="8.734375" style="3"/>
+    <col min="1039" max="1039" width="13.7890625" style="3" customWidth="1"/>
+    <col min="1040" max="1040" width="16.7890625" style="3" customWidth="1"/>
+    <col min="1041" max="1276" width="8.734375" style="3"/>
+    <col min="1277" max="1278" width="18.5234375" style="3" customWidth="1"/>
+    <col min="1279" max="1294" width="8.734375" style="3"/>
+    <col min="1295" max="1295" width="13.7890625" style="3" customWidth="1"/>
+    <col min="1296" max="1296" width="16.7890625" style="3" customWidth="1"/>
+    <col min="1297" max="1532" width="8.734375" style="3"/>
+    <col min="1533" max="1534" width="18.5234375" style="3" customWidth="1"/>
+    <col min="1535" max="1550" width="8.734375" style="3"/>
+    <col min="1551" max="1551" width="13.7890625" style="3" customWidth="1"/>
+    <col min="1552" max="1552" width="16.7890625" style="3" customWidth="1"/>
+    <col min="1553" max="1788" width="8.734375" style="3"/>
+    <col min="1789" max="1790" width="18.5234375" style="3" customWidth="1"/>
+    <col min="1791" max="1806" width="8.734375" style="3"/>
+    <col min="1807" max="1807" width="13.7890625" style="3" customWidth="1"/>
+    <col min="1808" max="1808" width="16.7890625" style="3" customWidth="1"/>
+    <col min="1809" max="2044" width="8.734375" style="3"/>
+    <col min="2045" max="2046" width="18.5234375" style="3" customWidth="1"/>
+    <col min="2047" max="2062" width="8.734375" style="3"/>
+    <col min="2063" max="2063" width="13.7890625" style="3" customWidth="1"/>
+    <col min="2064" max="2064" width="16.7890625" style="3" customWidth="1"/>
+    <col min="2065" max="2300" width="8.734375" style="3"/>
+    <col min="2301" max="2302" width="18.5234375" style="3" customWidth="1"/>
+    <col min="2303" max="2318" width="8.734375" style="3"/>
+    <col min="2319" max="2319" width="13.7890625" style="3" customWidth="1"/>
+    <col min="2320" max="2320" width="16.7890625" style="3" customWidth="1"/>
+    <col min="2321" max="2556" width="8.734375" style="3"/>
+    <col min="2557" max="2558" width="18.5234375" style="3" customWidth="1"/>
+    <col min="2559" max="2574" width="8.734375" style="3"/>
+    <col min="2575" max="2575" width="13.7890625" style="3" customWidth="1"/>
+    <col min="2576" max="2576" width="16.7890625" style="3" customWidth="1"/>
+    <col min="2577" max="2812" width="8.734375" style="3"/>
+    <col min="2813" max="2814" width="18.5234375" style="3" customWidth="1"/>
+    <col min="2815" max="2830" width="8.734375" style="3"/>
+    <col min="2831" max="2831" width="13.7890625" style="3" customWidth="1"/>
+    <col min="2832" max="2832" width="16.7890625" style="3" customWidth="1"/>
+    <col min="2833" max="3068" width="8.734375" style="3"/>
+    <col min="3069" max="3070" width="18.5234375" style="3" customWidth="1"/>
+    <col min="3071" max="3086" width="8.734375" style="3"/>
+    <col min="3087" max="3087" width="13.7890625" style="3" customWidth="1"/>
+    <col min="3088" max="3088" width="16.7890625" style="3" customWidth="1"/>
+    <col min="3089" max="3324" width="8.734375" style="3"/>
+    <col min="3325" max="3326" width="18.5234375" style="3" customWidth="1"/>
+    <col min="3327" max="3342" width="8.734375" style="3"/>
+    <col min="3343" max="3343" width="13.7890625" style="3" customWidth="1"/>
+    <col min="3344" max="3344" width="16.7890625" style="3" customWidth="1"/>
+    <col min="3345" max="3580" width="8.734375" style="3"/>
+    <col min="3581" max="3582" width="18.5234375" style="3" customWidth="1"/>
+    <col min="3583" max="3598" width="8.734375" style="3"/>
+    <col min="3599" max="3599" width="13.7890625" style="3" customWidth="1"/>
+    <col min="3600" max="3600" width="16.7890625" style="3" customWidth="1"/>
+    <col min="3601" max="3836" width="8.734375" style="3"/>
+    <col min="3837" max="3838" width="18.5234375" style="3" customWidth="1"/>
+    <col min="3839" max="3854" width="8.734375" style="3"/>
+    <col min="3855" max="3855" width="13.7890625" style="3" customWidth="1"/>
+    <col min="3856" max="3856" width="16.7890625" style="3" customWidth="1"/>
+    <col min="3857" max="4092" width="8.734375" style="3"/>
+    <col min="4093" max="4094" width="18.5234375" style="3" customWidth="1"/>
+    <col min="4095" max="4110" width="8.734375" style="3"/>
+    <col min="4111" max="4111" width="13.7890625" style="3" customWidth="1"/>
+    <col min="4112" max="4112" width="16.7890625" style="3" customWidth="1"/>
+    <col min="4113" max="4348" width="8.734375" style="3"/>
+    <col min="4349" max="4350" width="18.5234375" style="3" customWidth="1"/>
+    <col min="4351" max="4366" width="8.734375" style="3"/>
+    <col min="4367" max="4367" width="13.7890625" style="3" customWidth="1"/>
+    <col min="4368" max="4368" width="16.7890625" style="3" customWidth="1"/>
+    <col min="4369" max="4604" width="8.734375" style="3"/>
+    <col min="4605" max="4606" width="18.5234375" style="3" customWidth="1"/>
+    <col min="4607" max="4622" width="8.734375" style="3"/>
+    <col min="4623" max="4623" width="13.7890625" style="3" customWidth="1"/>
+    <col min="4624" max="4624" width="16.7890625" style="3" customWidth="1"/>
+    <col min="4625" max="4860" width="8.734375" style="3"/>
+    <col min="4861" max="4862" width="18.5234375" style="3" customWidth="1"/>
+    <col min="4863" max="4878" width="8.734375" style="3"/>
+    <col min="4879" max="4879" width="13.7890625" style="3" customWidth="1"/>
+    <col min="4880" max="4880" width="16.7890625" style="3" customWidth="1"/>
+    <col min="4881" max="5116" width="8.734375" style="3"/>
+    <col min="5117" max="5118" width="18.5234375" style="3" customWidth="1"/>
+    <col min="5119" max="5134" width="8.734375" style="3"/>
+    <col min="5135" max="5135" width="13.7890625" style="3" customWidth="1"/>
+    <col min="5136" max="5136" width="16.7890625" style="3" customWidth="1"/>
+    <col min="5137" max="5372" width="8.734375" style="3"/>
+    <col min="5373" max="5374" width="18.5234375" style="3" customWidth="1"/>
+    <col min="5375" max="5390" width="8.734375" style="3"/>
+    <col min="5391" max="5391" width="13.7890625" style="3" customWidth="1"/>
+    <col min="5392" max="5392" width="16.7890625" style="3" customWidth="1"/>
+    <col min="5393" max="5628" width="8.734375" style="3"/>
+    <col min="5629" max="5630" width="18.5234375" style="3" customWidth="1"/>
+    <col min="5631" max="5646" width="8.734375" style="3"/>
+    <col min="5647" max="5647" width="13.7890625" style="3" customWidth="1"/>
+    <col min="5648" max="5648" width="16.7890625" style="3" customWidth="1"/>
+    <col min="5649" max="5884" width="8.734375" style="3"/>
+    <col min="5885" max="5886" width="18.5234375" style="3" customWidth="1"/>
+    <col min="5887" max="5902" width="8.734375" style="3"/>
+    <col min="5903" max="5903" width="13.7890625" style="3" customWidth="1"/>
+    <col min="5904" max="5904" width="16.7890625" style="3" customWidth="1"/>
+    <col min="5905" max="6140" width="8.734375" style="3"/>
+    <col min="6141" max="6142" width="18.5234375" style="3" customWidth="1"/>
+    <col min="6143" max="6158" width="8.734375" style="3"/>
+    <col min="6159" max="6159" width="13.7890625" style="3" customWidth="1"/>
+    <col min="6160" max="6160" width="16.7890625" style="3" customWidth="1"/>
+    <col min="6161" max="6396" width="8.734375" style="3"/>
+    <col min="6397" max="6398" width="18.5234375" style="3" customWidth="1"/>
+    <col min="6399" max="6414" width="8.734375" style="3"/>
+    <col min="6415" max="6415" width="13.7890625" style="3" customWidth="1"/>
+    <col min="6416" max="6416" width="16.7890625" style="3" customWidth="1"/>
+    <col min="6417" max="6652" width="8.734375" style="3"/>
+    <col min="6653" max="6654" width="18.5234375" style="3" customWidth="1"/>
+    <col min="6655" max="6670" width="8.734375" style="3"/>
+    <col min="6671" max="6671" width="13.7890625" style="3" customWidth="1"/>
+    <col min="6672" max="6672" width="16.7890625" style="3" customWidth="1"/>
+    <col min="6673" max="6908" width="8.734375" style="3"/>
+    <col min="6909" max="6910" width="18.5234375" style="3" customWidth="1"/>
+    <col min="6911" max="6926" width="8.734375" style="3"/>
+    <col min="6927" max="6927" width="13.7890625" style="3" customWidth="1"/>
+    <col min="6928" max="6928" width="16.7890625" style="3" customWidth="1"/>
+    <col min="6929" max="7164" width="8.734375" style="3"/>
+    <col min="7165" max="7166" width="18.5234375" style="3" customWidth="1"/>
+    <col min="7167" max="7182" width="8.734375" style="3"/>
+    <col min="7183" max="7183" width="13.7890625" style="3" customWidth="1"/>
+    <col min="7184" max="7184" width="16.7890625" style="3" customWidth="1"/>
+    <col min="7185" max="7420" width="8.734375" style="3"/>
+    <col min="7421" max="7422" width="18.5234375" style="3" customWidth="1"/>
+    <col min="7423" max="7438" width="8.734375" style="3"/>
+    <col min="7439" max="7439" width="13.7890625" style="3" customWidth="1"/>
+    <col min="7440" max="7440" width="16.7890625" style="3" customWidth="1"/>
+    <col min="7441" max="7676" width="8.734375" style="3"/>
+    <col min="7677" max="7678" width="18.5234375" style="3" customWidth="1"/>
+    <col min="7679" max="7694" width="8.734375" style="3"/>
+    <col min="7695" max="7695" width="13.7890625" style="3" customWidth="1"/>
+    <col min="7696" max="7696" width="16.7890625" style="3" customWidth="1"/>
+    <col min="7697" max="7932" width="8.734375" style="3"/>
+    <col min="7933" max="7934" width="18.5234375" style="3" customWidth="1"/>
+    <col min="7935" max="7950" width="8.734375" style="3"/>
+    <col min="7951" max="7951" width="13.7890625" style="3" customWidth="1"/>
+    <col min="7952" max="7952" width="16.7890625" style="3" customWidth="1"/>
+    <col min="7953" max="8188" width="8.734375" style="3"/>
+    <col min="8189" max="8190" width="18.5234375" style="3" customWidth="1"/>
+    <col min="8191" max="8206" width="8.734375" style="3"/>
+    <col min="8207" max="8207" width="13.7890625" style="3" customWidth="1"/>
+    <col min="8208" max="8208" width="16.7890625" style="3" customWidth="1"/>
+    <col min="8209" max="8444" width="8.734375" style="3"/>
+    <col min="8445" max="8446" width="18.5234375" style="3" customWidth="1"/>
+    <col min="8447" max="8462" width="8.734375" style="3"/>
+    <col min="8463" max="8463" width="13.7890625" style="3" customWidth="1"/>
+    <col min="8464" max="8464" width="16.7890625" style="3" customWidth="1"/>
+    <col min="8465" max="8700" width="8.734375" style="3"/>
+    <col min="8701" max="8702" width="18.5234375" style="3" customWidth="1"/>
+    <col min="8703" max="8718" width="8.734375" style="3"/>
+    <col min="8719" max="8719" width="13.7890625" style="3" customWidth="1"/>
+    <col min="8720" max="8720" width="16.7890625" style="3" customWidth="1"/>
+    <col min="8721" max="8956" width="8.734375" style="3"/>
+    <col min="8957" max="8958" width="18.5234375" style="3" customWidth="1"/>
+    <col min="8959" max="8974" width="8.734375" style="3"/>
+    <col min="8975" max="8975" width="13.7890625" style="3" customWidth="1"/>
+    <col min="8976" max="8976" width="16.7890625" style="3" customWidth="1"/>
+    <col min="8977" max="9212" width="8.734375" style="3"/>
+    <col min="9213" max="9214" width="18.5234375" style="3" customWidth="1"/>
+    <col min="9215" max="9230" width="8.734375" style="3"/>
+    <col min="9231" max="9231" width="13.7890625" style="3" customWidth="1"/>
+    <col min="9232" max="9232" width="16.7890625" style="3" customWidth="1"/>
+    <col min="9233" max="9468" width="8.734375" style="3"/>
+    <col min="9469" max="9470" width="18.5234375" style="3" customWidth="1"/>
+    <col min="9471" max="9486" width="8.734375" style="3"/>
+    <col min="9487" max="9487" width="13.7890625" style="3" customWidth="1"/>
+    <col min="9488" max="9488" width="16.7890625" style="3" customWidth="1"/>
+    <col min="9489" max="9724" width="8.734375" style="3"/>
+    <col min="9725" max="9726" width="18.5234375" style="3" customWidth="1"/>
+    <col min="9727" max="9742" width="8.734375" style="3"/>
+    <col min="9743" max="9743" width="13.7890625" style="3" customWidth="1"/>
+    <col min="9744" max="9744" width="16.7890625" style="3" customWidth="1"/>
+    <col min="9745" max="9980" width="8.734375" style="3"/>
+    <col min="9981" max="9982" width="18.5234375" style="3" customWidth="1"/>
+    <col min="9983" max="9998" width="8.734375" style="3"/>
+    <col min="9999" max="9999" width="13.7890625" style="3" customWidth="1"/>
+    <col min="10000" max="10000" width="16.7890625" style="3" customWidth="1"/>
+    <col min="10001" max="10236" width="8.734375" style="3"/>
+    <col min="10237" max="10238" width="18.5234375" style="3" customWidth="1"/>
+    <col min="10239" max="10254" width="8.734375" style="3"/>
+    <col min="10255" max="10255" width="13.7890625" style="3" customWidth="1"/>
+    <col min="10256" max="10256" width="16.7890625" style="3" customWidth="1"/>
+    <col min="10257" max="10492" width="8.734375" style="3"/>
+    <col min="10493" max="10494" width="18.5234375" style="3" customWidth="1"/>
+    <col min="10495" max="10510" width="8.734375" style="3"/>
+    <col min="10511" max="10511" width="13.7890625" style="3" customWidth="1"/>
+    <col min="10512" max="10512" width="16.7890625" style="3" customWidth="1"/>
+    <col min="10513" max="10748" width="8.734375" style="3"/>
+    <col min="10749" max="10750" width="18.5234375" style="3" customWidth="1"/>
+    <col min="10751" max="10766" width="8.734375" style="3"/>
+    <col min="10767" max="10767" width="13.7890625" style="3" customWidth="1"/>
+    <col min="10768" max="10768" width="16.7890625" style="3" customWidth="1"/>
+    <col min="10769" max="11004" width="8.734375" style="3"/>
+    <col min="11005" max="11006" width="18.5234375" style="3" customWidth="1"/>
+    <col min="11007" max="11022" width="8.734375" style="3"/>
+    <col min="11023" max="11023" width="13.7890625" style="3" customWidth="1"/>
+    <col min="11024" max="11024" width="16.7890625" style="3" customWidth="1"/>
+    <col min="11025" max="11260" width="8.734375" style="3"/>
+    <col min="11261" max="11262" width="18.5234375" style="3" customWidth="1"/>
+    <col min="11263" max="11278" width="8.734375" style="3"/>
+    <col min="11279" max="11279" width="13.7890625" style="3" customWidth="1"/>
+    <col min="11280" max="11280" width="16.7890625" style="3" customWidth="1"/>
+    <col min="11281" max="11516" width="8.734375" style="3"/>
+    <col min="11517" max="11518" width="18.5234375" style="3" customWidth="1"/>
+    <col min="11519" max="11534" width="8.734375" style="3"/>
+    <col min="11535" max="11535" width="13.7890625" style="3" customWidth="1"/>
+    <col min="11536" max="11536" width="16.7890625" style="3" customWidth="1"/>
+    <col min="11537" max="11772" width="8.734375" style="3"/>
+    <col min="11773" max="11774" width="18.5234375" style="3" customWidth="1"/>
+    <col min="11775" max="11790" width="8.734375" style="3"/>
+    <col min="11791" max="11791" width="13.7890625" style="3" customWidth="1"/>
+    <col min="11792" max="11792" width="16.7890625" style="3" customWidth="1"/>
+    <col min="11793" max="12028" width="8.734375" style="3"/>
+    <col min="12029" max="12030" width="18.5234375" style="3" customWidth="1"/>
+    <col min="12031" max="12046" width="8.734375" style="3"/>
+    <col min="12047" max="12047" width="13.7890625" style="3" customWidth="1"/>
+    <col min="12048" max="12048" width="16.7890625" style="3" customWidth="1"/>
+    <col min="12049" max="12284" width="8.734375" style="3"/>
+    <col min="12285" max="12286" width="18.5234375" style="3" customWidth="1"/>
+    <col min="12287" max="12302" width="8.734375" style="3"/>
+    <col min="12303" max="12303" width="13.7890625" style="3" customWidth="1"/>
+    <col min="12304" max="12304" width="16.7890625" style="3" customWidth="1"/>
+    <col min="12305" max="12540" width="8.734375" style="3"/>
+    <col min="12541" max="12542" width="18.5234375" style="3" customWidth="1"/>
+    <col min="12543" max="12558" width="8.734375" style="3"/>
+    <col min="12559" max="12559" width="13.7890625" style="3" customWidth="1"/>
+    <col min="12560" max="12560" width="16.7890625" style="3" customWidth="1"/>
+    <col min="12561" max="12796" width="8.734375" style="3"/>
+    <col min="12797" max="12798" width="18.5234375" style="3" customWidth="1"/>
+    <col min="12799" max="12814" width="8.734375" style="3"/>
+    <col min="12815" max="12815" width="13.7890625" style="3" customWidth="1"/>
+    <col min="12816" max="12816" width="16.7890625" style="3" customWidth="1"/>
+    <col min="12817" max="13052" width="8.734375" style="3"/>
+    <col min="13053" max="13054" width="18.5234375" style="3" customWidth="1"/>
+    <col min="13055" max="13070" width="8.734375" style="3"/>
+    <col min="13071" max="13071" width="13.7890625" style="3" customWidth="1"/>
+    <col min="13072" max="13072" width="16.7890625" style="3" customWidth="1"/>
+    <col min="13073" max="13308" width="8.734375" style="3"/>
+    <col min="13309" max="13310" width="18.5234375" style="3" customWidth="1"/>
+    <col min="13311" max="13326" width="8.734375" style="3"/>
+    <col min="13327" max="13327" width="13.7890625" style="3" customWidth="1"/>
+    <col min="13328" max="13328" width="16.7890625" style="3" customWidth="1"/>
+    <col min="13329" max="13564" width="8.734375" style="3"/>
+    <col min="13565" max="13566" width="18.5234375" style="3" customWidth="1"/>
+    <col min="13567" max="13582" width="8.734375" style="3"/>
+    <col min="13583" max="13583" width="13.7890625" style="3" customWidth="1"/>
+    <col min="13584" max="13584" width="16.7890625" style="3" customWidth="1"/>
+    <col min="13585" max="13820" width="8.734375" style="3"/>
+    <col min="13821" max="13822" width="18.5234375" style="3" customWidth="1"/>
+    <col min="13823" max="13838" width="8.734375" style="3"/>
+    <col min="13839" max="13839" width="13.7890625" style="3" customWidth="1"/>
+    <col min="13840" max="13840" width="16.7890625" style="3" customWidth="1"/>
+    <col min="13841" max="14076" width="8.734375" style="3"/>
+    <col min="14077" max="14078" width="18.5234375" style="3" customWidth="1"/>
+    <col min="14079" max="14094" width="8.734375" style="3"/>
+    <col min="14095" max="14095" width="13.7890625" style="3" customWidth="1"/>
+    <col min="14096" max="14096" width="16.7890625" style="3" customWidth="1"/>
+    <col min="14097" max="14332" width="8.734375" style="3"/>
+    <col min="14333" max="14334" width="18.5234375" style="3" customWidth="1"/>
+    <col min="14335" max="14350" width="8.734375" style="3"/>
+    <col min="14351" max="14351" width="13.7890625" style="3" customWidth="1"/>
+    <col min="14352" max="14352" width="16.7890625" style="3" customWidth="1"/>
+    <col min="14353" max="14588" width="8.734375" style="3"/>
+    <col min="14589" max="14590" width="18.5234375" style="3" customWidth="1"/>
+    <col min="14591" max="14606" width="8.734375" style="3"/>
+    <col min="14607" max="14607" width="13.7890625" style="3" customWidth="1"/>
+    <col min="14608" max="14608" width="16.7890625" style="3" customWidth="1"/>
+    <col min="14609" max="14844" width="8.734375" style="3"/>
+    <col min="14845" max="14846" width="18.5234375" style="3" customWidth="1"/>
+    <col min="14847" max="14862" width="8.734375" style="3"/>
+    <col min="14863" max="14863" width="13.7890625" style="3" customWidth="1"/>
+    <col min="14864" max="14864" width="16.7890625" style="3" customWidth="1"/>
+    <col min="14865" max="15100" width="8.734375" style="3"/>
+    <col min="15101" max="15102" width="18.5234375" style="3" customWidth="1"/>
+    <col min="15103" max="15118" width="8.734375" style="3"/>
+    <col min="15119" max="15119" width="13.7890625" style="3" customWidth="1"/>
+    <col min="15120" max="15120" width="16.7890625" style="3" customWidth="1"/>
+    <col min="15121" max="15356" width="8.734375" style="3"/>
+    <col min="15357" max="15358" width="18.5234375" style="3" customWidth="1"/>
+    <col min="15359" max="15374" width="8.734375" style="3"/>
+    <col min="15375" max="15375" width="13.7890625" style="3" customWidth="1"/>
+    <col min="15376" max="15376" width="16.7890625" style="3" customWidth="1"/>
+    <col min="15377" max="15612" width="8.734375" style="3"/>
+    <col min="15613" max="15614" width="18.5234375" style="3" customWidth="1"/>
+    <col min="15615" max="15630" width="8.734375" style="3"/>
+    <col min="15631" max="15631" width="13.7890625" style="3" customWidth="1"/>
+    <col min="15632" max="15632" width="16.7890625" style="3" customWidth="1"/>
+    <col min="15633" max="15868" width="8.734375" style="3"/>
+    <col min="15869" max="15870" width="18.5234375" style="3" customWidth="1"/>
+    <col min="15871" max="15886" width="8.734375" style="3"/>
+    <col min="15887" max="15887" width="13.7890625" style="3" customWidth="1"/>
+    <col min="15888" max="15888" width="16.7890625" style="3" customWidth="1"/>
+    <col min="15889" max="16124" width="8.734375" style="3"/>
+    <col min="16125" max="16126" width="18.5234375" style="3" customWidth="1"/>
+    <col min="16127" max="16142" width="8.734375" style="3"/>
+    <col min="16143" max="16143" width="13.7890625" style="3" customWidth="1"/>
+    <col min="16144" max="16144" width="16.7890625" style="3" customWidth="1"/>
+    <col min="16145" max="16384" width="8.734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="1" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" s="1" customFormat="1" ht="135.30000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -5886,7 +5886,7 @@
       <c r="AY2" s="7"/>
       <c r="AZ2" s="7"/>
     </row>
-    <row r="3" spans="1:54" s="1" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="1" customFormat="1" ht="49.2" x14ac:dyDescent="0.4">
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="14" t="s">
         <v>102</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="14" t="s">
         <v>103</v>
       </c>
@@ -6236,7 +6236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="14" t="s">
         <v>104</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>11.77</v>
       </c>
     </row>
-    <row r="7" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="14"/>
       <c r="B7" s="19"/>
       <c r="C7" s="14"/>
@@ -6451,7 +6451,7 @@
       <c r="BA7" s="15"/>
       <c r="BB7" s="15"/>
     </row>
-    <row r="8" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="14" t="s">
         <v>52</v>
       </c>
@@ -6527,7 +6527,7 @@
       <c r="BA8" s="15"/>
       <c r="BB8" s="15"/>
     </row>
-    <row r="9" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9"/>
       <c r="C9"/>
       <c r="E9"/>
@@ -6569,7 +6569,7 @@
       <c r="AY9" s="7"/>
       <c r="AZ9" s="7"/>
     </row>
-    <row r="10" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>105</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>1113.3399999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="14" t="s">
         <v>106</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>135.88</v>
       </c>
     </row>
-    <row r="12" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="14" t="s">
         <v>107</v>
       </c>
@@ -7035,7 +7035,7 @@
         <v>270.06</v>
       </c>
     </row>
-    <row r="13" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14" t="s">
         <v>108</v>
       </c>
@@ -7189,7 +7189,7 @@
         <v>213.96999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="14" t="s">
         <v>109</v>
       </c>
@@ -7344,9 +7344,9 @@
         <v>439.87</v>
       </c>
     </row>
-    <row r="15" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15">
@@ -7499,7 +7499,7 @@
         <v>394.01000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="14" t="s">
         <v>105</v>
       </c>
@@ -7654,9 +7654,9 @@
         <v>919.91</v>
       </c>
     </row>
-    <row r="17" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17">
@@ -7809,7 +7809,7 @@
         <v>283.45000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="14" t="s">
         <v>112</v>
       </c>
@@ -7964,7 +7964,7 @@
         <v>427.93999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="14" t="s">
         <v>113</v>
       </c>
@@ -8119,7 +8119,7 @@
         <v>202.12</v>
       </c>
     </row>
-    <row r="20" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="14" t="s">
         <v>114</v>
       </c>
@@ -8274,7 +8274,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="14" t="s">
         <v>115</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>441.33</v>
       </c>
     </row>
-    <row r="22" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="14" t="s">
         <v>116</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>225.81999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="14"/>
       <c r="B23" s="9"/>
       <c r="C23"/>
@@ -8627,7 +8627,7 @@
       <c r="AY23" s="7"/>
       <c r="AZ23" s="7"/>
     </row>
-    <row r="24" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="14"/>
       <c r="B24" s="9"/>
       <c r="C24"/>
@@ -8670,7 +8670,7 @@
       <c r="AY24" s="7"/>
       <c r="AZ24" s="7"/>
     </row>
-    <row r="25" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="14"/>
       <c r="B25" s="9"/>
       <c r="C25"/>
@@ -8713,7 +8713,7 @@
       <c r="AY25" s="7"/>
       <c r="AZ25" s="7"/>
     </row>
-    <row r="26" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="14"/>
       <c r="B26" s="9"/>
       <c r="C26"/>
@@ -8756,7 +8756,7 @@
       <c r="AY26" s="7"/>
       <c r="AZ26" s="7"/>
     </row>
-    <row r="27" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="14"/>
       <c r="B27" s="9"/>
       <c r="C27"/>
@@ -8799,7 +8799,7 @@
       <c r="AY27" s="7"/>
       <c r="AZ27" s="7"/>
     </row>
-    <row r="28" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="14"/>
       <c r="B28" s="9"/>
       <c r="C28"/>
@@ -8842,7 +8842,7 @@
       <c r="AY28" s="7"/>
       <c r="AZ28" s="7"/>
     </row>
-    <row r="29" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
@@ -8882,7 +8882,7 @@
       <c r="AY29" s="7"/>
       <c r="AZ29" s="7"/>
     </row>
-    <row r="30" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
@@ -8922,7 +8922,7 @@
       <c r="AY30" s="7"/>
       <c r="AZ30" s="7"/>
     </row>
-    <row r="31" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
@@ -8962,7 +8962,7 @@
       <c r="AY31" s="7"/>
       <c r="AZ31" s="7"/>
     </row>
-    <row r="32" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:54" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F32"/>
       <c r="G32"/>
       <c r="H32"/>
@@ -9000,7 +9000,7 @@
       <c r="AY32" s="7"/>
       <c r="AZ32" s="7"/>
     </row>
-    <row r="33" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33"/>
@@ -9038,7 +9038,7 @@
       <c r="AY33" s="7"/>
       <c r="AZ33" s="7"/>
     </row>
-    <row r="34" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F34"/>
       <c r="G34"/>
       <c r="H34"/>
@@ -9076,7 +9076,7 @@
       <c r="AY34" s="7"/>
       <c r="AZ34" s="7"/>
     </row>
-    <row r="35" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F35"/>
       <c r="G35"/>
       <c r="H35"/>
@@ -9114,7 +9114,7 @@
       <c r="AY35" s="7"/>
       <c r="AZ35" s="7"/>
     </row>
-    <row r="36" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F36"/>
       <c r="G36"/>
       <c r="H36"/>
@@ -9152,7 +9152,7 @@
       <c r="AY36" s="7"/>
       <c r="AZ36" s="7"/>
     </row>
-    <row r="37" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F37"/>
       <c r="G37"/>
       <c r="H37"/>
@@ -9190,7 +9190,7 @@
       <c r="AY37" s="7"/>
       <c r="AZ37" s="7"/>
     </row>
-    <row r="38" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F38"/>
       <c r="G38"/>
       <c r="H38"/>
@@ -9228,7 +9228,7 @@
       <c r="AY38" s="7"/>
       <c r="AZ38" s="7"/>
     </row>
-    <row r="39" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F39"/>
       <c r="G39"/>
       <c r="H39"/>
@@ -9266,7 +9266,7 @@
       <c r="AY39" s="7"/>
       <c r="AZ39" s="7"/>
     </row>
-    <row r="40" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F40"/>
       <c r="G40"/>
       <c r="H40"/>
@@ -9304,7 +9304,7 @@
       <c r="AY40" s="7"/>
       <c r="AZ40" s="7"/>
     </row>
-    <row r="41" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41"/>
@@ -9342,7 +9342,7 @@
       <c r="AY41" s="7"/>
       <c r="AZ41" s="7"/>
     </row>
-    <row r="42" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42"/>
@@ -9380,7 +9380,7 @@
       <c r="AY42" s="7"/>
       <c r="AZ42" s="7"/>
     </row>
-    <row r="43" spans="6:52" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="6:52" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
@@ -9415,7 +9415,7 @@
       <c r="AQ43" s="6"/>
       <c r="AR43" s="6"/>
     </row>
-    <row r="44" spans="6:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:52" x14ac:dyDescent="0.4">
       <c r="AB44" s="6"/>
       <c r="AC44" s="6"/>
       <c r="AD44" s="6"/>
@@ -9430,7 +9430,7 @@
       <c r="AQ44" s="6"/>
       <c r="AR44" s="6"/>
     </row>
-    <row r="45" spans="6:52" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:52" x14ac:dyDescent="0.4">
       <c r="AB45" s="6"/>
       <c r="AC45" s="6"/>
       <c r="AD45" s="6"/>
@@ -9445,7 +9445,7 @@
       <c r="AQ45" s="6"/>
       <c r="AR45" s="6"/>
     </row>
-    <row r="46" spans="6:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:52" x14ac:dyDescent="0.4">
       <c r="AB46" s="6"/>
       <c r="AC46" s="6"/>
       <c r="AD46" s="6"/>
@@ -9460,7 +9460,7 @@
       <c r="AQ46" s="6"/>
       <c r="AR46" s="6"/>
     </row>
-    <row r="47" spans="6:52" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:52" x14ac:dyDescent="0.4">
       <c r="AB47" s="6"/>
       <c r="AC47" s="6"/>
       <c r="AD47" s="6"/>
@@ -9475,7 +9475,7 @@
       <c r="AQ47" s="6"/>
       <c r="AR47" s="6"/>
     </row>
-    <row r="48" spans="6:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:52" x14ac:dyDescent="0.4">
       <c r="AB48" s="6"/>
       <c r="AC48" s="6"/>
       <c r="AD48" s="6"/>
@@ -9490,7 +9490,7 @@
       <c r="AQ48" s="6"/>
       <c r="AR48" s="6"/>
     </row>
-    <row r="49" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="49" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB49" s="6"/>
       <c r="AC49" s="6"/>
       <c r="AD49" s="6"/>
@@ -9505,7 +9505,7 @@
       <c r="AQ49" s="6"/>
       <c r="AR49" s="6"/>
     </row>
-    <row r="50" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="50" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB50" s="6"/>
       <c r="AC50" s="6"/>
       <c r="AD50" s="6"/>
@@ -9520,7 +9520,7 @@
       <c r="AQ50" s="6"/>
       <c r="AR50" s="6"/>
     </row>
-    <row r="51" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="51" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB51" s="6"/>
       <c r="AC51" s="6"/>
       <c r="AD51" s="6"/>
@@ -9535,7 +9535,7 @@
       <c r="AQ51" s="6"/>
       <c r="AR51" s="6"/>
     </row>
-    <row r="52" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="52" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB52" s="6"/>
       <c r="AC52" s="6"/>
       <c r="AD52" s="6"/>
@@ -9550,7 +9550,7 @@
       <c r="AQ52" s="6"/>
       <c r="AR52" s="6"/>
     </row>
-    <row r="53" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="53" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB53" s="6"/>
       <c r="AC53" s="6"/>
       <c r="AD53" s="6"/>
@@ -9565,7 +9565,7 @@
       <c r="AQ53" s="6"/>
       <c r="AR53" s="6"/>
     </row>
-    <row r="54" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="54" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB54" s="6"/>
       <c r="AC54" s="6"/>
       <c r="AD54" s="6"/>
@@ -9580,7 +9580,7 @@
       <c r="AQ54" s="6"/>
       <c r="AR54" s="6"/>
     </row>
-    <row r="55" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="55" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB55" s="6"/>
       <c r="AC55" s="6"/>
       <c r="AD55" s="6"/>
@@ -9595,7 +9595,7 @@
       <c r="AQ55" s="6"/>
       <c r="AR55" s="6"/>
     </row>
-    <row r="56" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="56" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB56" s="6"/>
       <c r="AC56" s="6"/>
       <c r="AD56" s="6"/>
@@ -9610,7 +9610,7 @@
       <c r="AQ56" s="6"/>
       <c r="AR56" s="6"/>
     </row>
-    <row r="57" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="57" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB57" s="6"/>
       <c r="AC57" s="6"/>
       <c r="AD57" s="6"/>
@@ -9625,7 +9625,7 @@
       <c r="AQ57" s="6"/>
       <c r="AR57" s="6"/>
     </row>
-    <row r="58" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="58" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB58" s="6"/>
       <c r="AC58" s="6"/>
       <c r="AD58" s="6"/>
@@ -9640,7 +9640,7 @@
       <c r="AQ58" s="6"/>
       <c r="AR58" s="6"/>
     </row>
-    <row r="59" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="59" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB59" s="6"/>
       <c r="AC59" s="6"/>
       <c r="AD59" s="6"/>
@@ -9655,7 +9655,7 @@
       <c r="AQ59" s="6"/>
       <c r="AR59" s="6"/>
     </row>
-    <row r="60" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="60" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB60" s="6"/>
       <c r="AC60" s="6"/>
       <c r="AD60" s="6"/>
@@ -9670,7 +9670,7 @@
       <c r="AQ60" s="6"/>
       <c r="AR60" s="6"/>
     </row>
-    <row r="61" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="61" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB61" s="6"/>
       <c r="AC61" s="6"/>
       <c r="AD61" s="6"/>
@@ -9685,7 +9685,7 @@
       <c r="AQ61" s="6"/>
       <c r="AR61" s="6"/>
     </row>
-    <row r="62" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="62" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB62" s="6"/>
       <c r="AC62" s="6"/>
       <c r="AD62" s="6"/>
@@ -9700,7 +9700,7 @@
       <c r="AQ62" s="6"/>
       <c r="AR62" s="6"/>
     </row>
-    <row r="63" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="63" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB63" s="6"/>
       <c r="AC63" s="6"/>
       <c r="AD63" s="6"/>
@@ -9715,7 +9715,7 @@
       <c r="AQ63" s="6"/>
       <c r="AR63" s="6"/>
     </row>
-    <row r="64" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="64" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB64" s="6"/>
       <c r="AC64" s="6"/>
       <c r="AD64" s="6"/>
@@ -9730,7 +9730,7 @@
       <c r="AQ64" s="6"/>
       <c r="AR64" s="6"/>
     </row>
-    <row r="65" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="65" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB65" s="6"/>
       <c r="AC65" s="6"/>
       <c r="AD65" s="6"/>
@@ -9745,7 +9745,7 @@
       <c r="AQ65" s="6"/>
       <c r="AR65" s="6"/>
     </row>
-    <row r="66" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="66" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB66" s="6"/>
       <c r="AC66" s="6"/>
       <c r="AD66" s="6"/>
@@ -9760,7 +9760,7 @@
       <c r="AQ66" s="6"/>
       <c r="AR66" s="6"/>
     </row>
-    <row r="67" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="67" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB67" s="6"/>
       <c r="AC67" s="6"/>
       <c r="AD67" s="6"/>
@@ -9775,7 +9775,7 @@
       <c r="AQ67" s="6"/>
       <c r="AR67" s="6"/>
     </row>
-    <row r="68" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="68" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB68" s="6"/>
       <c r="AC68" s="6"/>
       <c r="AD68" s="6"/>
@@ -9790,7 +9790,7 @@
       <c r="AQ68" s="6"/>
       <c r="AR68" s="6"/>
     </row>
-    <row r="69" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="69" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB69" s="6"/>
       <c r="AC69" s="6"/>
       <c r="AD69" s="6"/>
@@ -9805,7 +9805,7 @@
       <c r="AQ69" s="6"/>
       <c r="AR69" s="6"/>
     </row>
-    <row r="70" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="70" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB70" s="6"/>
       <c r="AC70" s="6"/>
       <c r="AD70" s="6"/>
@@ -9820,7 +9820,7 @@
       <c r="AQ70" s="6"/>
       <c r="AR70" s="6"/>
     </row>
-    <row r="71" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="71" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB71" s="6"/>
       <c r="AC71" s="6"/>
       <c r="AD71" s="6"/>
@@ -9835,7 +9835,7 @@
       <c r="AQ71" s="6"/>
       <c r="AR71" s="6"/>
     </row>
-    <row r="72" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="72" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB72" s="6"/>
       <c r="AC72" s="6"/>
       <c r="AD72" s="6"/>
@@ -9850,7 +9850,7 @@
       <c r="AQ72" s="6"/>
       <c r="AR72" s="6"/>
     </row>
-    <row r="73" spans="28:44" x14ac:dyDescent="0.25">
+    <row r="73" spans="28:44" x14ac:dyDescent="0.4">
       <c r="AB73" s="6"/>
       <c r="AC73" s="6"/>
       <c r="AD73" s="6"/>
@@ -9988,12 +9988,12 @@
       <selection activeCell="A7" sqref="A1:K56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7890625" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10008,333 +10008,333 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="35.26953125" style="3" customWidth="1"/>
-    <col min="2" max="19" width="10.7265625" style="3" customWidth="1"/>
-    <col min="20" max="21" width="10.7265625" style="4" customWidth="1"/>
-    <col min="22" max="23" width="10.7265625" style="3" customWidth="1"/>
-    <col min="24" max="30" width="8.7265625" style="3"/>
-    <col min="31" max="31" width="12.7265625" style="3" customWidth="1"/>
-    <col min="32" max="234" width="8.7265625" style="3"/>
-    <col min="235" max="236" width="18.54296875" style="3" customWidth="1"/>
-    <col min="237" max="252" width="8.7265625" style="3"/>
-    <col min="253" max="253" width="13.81640625" style="3" customWidth="1"/>
-    <col min="254" max="254" width="16.81640625" style="3" customWidth="1"/>
-    <col min="255" max="490" width="8.7265625" style="3"/>
-    <col min="491" max="492" width="18.54296875" style="3" customWidth="1"/>
-    <col min="493" max="508" width="8.7265625" style="3"/>
-    <col min="509" max="509" width="13.81640625" style="3" customWidth="1"/>
-    <col min="510" max="510" width="16.81640625" style="3" customWidth="1"/>
-    <col min="511" max="746" width="8.7265625" style="3"/>
-    <col min="747" max="748" width="18.54296875" style="3" customWidth="1"/>
-    <col min="749" max="764" width="8.7265625" style="3"/>
-    <col min="765" max="765" width="13.81640625" style="3" customWidth="1"/>
-    <col min="766" max="766" width="16.81640625" style="3" customWidth="1"/>
-    <col min="767" max="1002" width="8.7265625" style="3"/>
-    <col min="1003" max="1004" width="18.54296875" style="3" customWidth="1"/>
-    <col min="1005" max="1020" width="8.7265625" style="3"/>
-    <col min="1021" max="1021" width="13.81640625" style="3" customWidth="1"/>
-    <col min="1022" max="1022" width="16.81640625" style="3" customWidth="1"/>
-    <col min="1023" max="1258" width="8.7265625" style="3"/>
-    <col min="1259" max="1260" width="18.54296875" style="3" customWidth="1"/>
-    <col min="1261" max="1276" width="8.7265625" style="3"/>
-    <col min="1277" max="1277" width="13.81640625" style="3" customWidth="1"/>
-    <col min="1278" max="1278" width="16.81640625" style="3" customWidth="1"/>
-    <col min="1279" max="1514" width="8.7265625" style="3"/>
-    <col min="1515" max="1516" width="18.54296875" style="3" customWidth="1"/>
-    <col min="1517" max="1532" width="8.7265625" style="3"/>
-    <col min="1533" max="1533" width="13.81640625" style="3" customWidth="1"/>
-    <col min="1534" max="1534" width="16.81640625" style="3" customWidth="1"/>
-    <col min="1535" max="1770" width="8.7265625" style="3"/>
-    <col min="1771" max="1772" width="18.54296875" style="3" customWidth="1"/>
-    <col min="1773" max="1788" width="8.7265625" style="3"/>
-    <col min="1789" max="1789" width="13.81640625" style="3" customWidth="1"/>
-    <col min="1790" max="1790" width="16.81640625" style="3" customWidth="1"/>
-    <col min="1791" max="2026" width="8.7265625" style="3"/>
-    <col min="2027" max="2028" width="18.54296875" style="3" customWidth="1"/>
-    <col min="2029" max="2044" width="8.7265625" style="3"/>
-    <col min="2045" max="2045" width="13.81640625" style="3" customWidth="1"/>
-    <col min="2046" max="2046" width="16.81640625" style="3" customWidth="1"/>
-    <col min="2047" max="2282" width="8.7265625" style="3"/>
-    <col min="2283" max="2284" width="18.54296875" style="3" customWidth="1"/>
-    <col min="2285" max="2300" width="8.7265625" style="3"/>
-    <col min="2301" max="2301" width="13.81640625" style="3" customWidth="1"/>
-    <col min="2302" max="2302" width="16.81640625" style="3" customWidth="1"/>
-    <col min="2303" max="2538" width="8.7265625" style="3"/>
-    <col min="2539" max="2540" width="18.54296875" style="3" customWidth="1"/>
-    <col min="2541" max="2556" width="8.7265625" style="3"/>
-    <col min="2557" max="2557" width="13.81640625" style="3" customWidth="1"/>
-    <col min="2558" max="2558" width="16.81640625" style="3" customWidth="1"/>
-    <col min="2559" max="2794" width="8.7265625" style="3"/>
-    <col min="2795" max="2796" width="18.54296875" style="3" customWidth="1"/>
-    <col min="2797" max="2812" width="8.7265625" style="3"/>
-    <col min="2813" max="2813" width="13.81640625" style="3" customWidth="1"/>
-    <col min="2814" max="2814" width="16.81640625" style="3" customWidth="1"/>
-    <col min="2815" max="3050" width="8.7265625" style="3"/>
-    <col min="3051" max="3052" width="18.54296875" style="3" customWidth="1"/>
-    <col min="3053" max="3068" width="8.7265625" style="3"/>
-    <col min="3069" max="3069" width="13.81640625" style="3" customWidth="1"/>
-    <col min="3070" max="3070" width="16.81640625" style="3" customWidth="1"/>
-    <col min="3071" max="3306" width="8.7265625" style="3"/>
-    <col min="3307" max="3308" width="18.54296875" style="3" customWidth="1"/>
-    <col min="3309" max="3324" width="8.7265625" style="3"/>
-    <col min="3325" max="3325" width="13.81640625" style="3" customWidth="1"/>
-    <col min="3326" max="3326" width="16.81640625" style="3" customWidth="1"/>
-    <col min="3327" max="3562" width="8.7265625" style="3"/>
-    <col min="3563" max="3564" width="18.54296875" style="3" customWidth="1"/>
-    <col min="3565" max="3580" width="8.7265625" style="3"/>
-    <col min="3581" max="3581" width="13.81640625" style="3" customWidth="1"/>
-    <col min="3582" max="3582" width="16.81640625" style="3" customWidth="1"/>
-    <col min="3583" max="3818" width="8.7265625" style="3"/>
-    <col min="3819" max="3820" width="18.54296875" style="3" customWidth="1"/>
-    <col min="3821" max="3836" width="8.7265625" style="3"/>
-    <col min="3837" max="3837" width="13.81640625" style="3" customWidth="1"/>
-    <col min="3838" max="3838" width="16.81640625" style="3" customWidth="1"/>
-    <col min="3839" max="4074" width="8.7265625" style="3"/>
-    <col min="4075" max="4076" width="18.54296875" style="3" customWidth="1"/>
-    <col min="4077" max="4092" width="8.7265625" style="3"/>
-    <col min="4093" max="4093" width="13.81640625" style="3" customWidth="1"/>
-    <col min="4094" max="4094" width="16.81640625" style="3" customWidth="1"/>
-    <col min="4095" max="4330" width="8.7265625" style="3"/>
-    <col min="4331" max="4332" width="18.54296875" style="3" customWidth="1"/>
-    <col min="4333" max="4348" width="8.7265625" style="3"/>
-    <col min="4349" max="4349" width="13.81640625" style="3" customWidth="1"/>
-    <col min="4350" max="4350" width="16.81640625" style="3" customWidth="1"/>
-    <col min="4351" max="4586" width="8.7265625" style="3"/>
-    <col min="4587" max="4588" width="18.54296875" style="3" customWidth="1"/>
-    <col min="4589" max="4604" width="8.7265625" style="3"/>
-    <col min="4605" max="4605" width="13.81640625" style="3" customWidth="1"/>
-    <col min="4606" max="4606" width="16.81640625" style="3" customWidth="1"/>
-    <col min="4607" max="4842" width="8.7265625" style="3"/>
-    <col min="4843" max="4844" width="18.54296875" style="3" customWidth="1"/>
-    <col min="4845" max="4860" width="8.7265625" style="3"/>
-    <col min="4861" max="4861" width="13.81640625" style="3" customWidth="1"/>
-    <col min="4862" max="4862" width="16.81640625" style="3" customWidth="1"/>
-    <col min="4863" max="5098" width="8.7265625" style="3"/>
-    <col min="5099" max="5100" width="18.54296875" style="3" customWidth="1"/>
-    <col min="5101" max="5116" width="8.7265625" style="3"/>
-    <col min="5117" max="5117" width="13.81640625" style="3" customWidth="1"/>
-    <col min="5118" max="5118" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5119" max="5354" width="8.7265625" style="3"/>
-    <col min="5355" max="5356" width="18.54296875" style="3" customWidth="1"/>
-    <col min="5357" max="5372" width="8.7265625" style="3"/>
-    <col min="5373" max="5373" width="13.81640625" style="3" customWidth="1"/>
-    <col min="5374" max="5374" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5375" max="5610" width="8.7265625" style="3"/>
-    <col min="5611" max="5612" width="18.54296875" style="3" customWidth="1"/>
-    <col min="5613" max="5628" width="8.7265625" style="3"/>
-    <col min="5629" max="5629" width="13.81640625" style="3" customWidth="1"/>
-    <col min="5630" max="5630" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5631" max="5866" width="8.7265625" style="3"/>
-    <col min="5867" max="5868" width="18.54296875" style="3" customWidth="1"/>
-    <col min="5869" max="5884" width="8.7265625" style="3"/>
-    <col min="5885" max="5885" width="13.81640625" style="3" customWidth="1"/>
-    <col min="5886" max="5886" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5887" max="6122" width="8.7265625" style="3"/>
-    <col min="6123" max="6124" width="18.54296875" style="3" customWidth="1"/>
-    <col min="6125" max="6140" width="8.7265625" style="3"/>
-    <col min="6141" max="6141" width="13.81640625" style="3" customWidth="1"/>
-    <col min="6142" max="6142" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6143" max="6378" width="8.7265625" style="3"/>
-    <col min="6379" max="6380" width="18.54296875" style="3" customWidth="1"/>
-    <col min="6381" max="6396" width="8.7265625" style="3"/>
-    <col min="6397" max="6397" width="13.81640625" style="3" customWidth="1"/>
-    <col min="6398" max="6398" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6399" max="6634" width="8.7265625" style="3"/>
-    <col min="6635" max="6636" width="18.54296875" style="3" customWidth="1"/>
-    <col min="6637" max="6652" width="8.7265625" style="3"/>
-    <col min="6653" max="6653" width="13.81640625" style="3" customWidth="1"/>
-    <col min="6654" max="6654" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6655" max="6890" width="8.7265625" style="3"/>
-    <col min="6891" max="6892" width="18.54296875" style="3" customWidth="1"/>
-    <col min="6893" max="6908" width="8.7265625" style="3"/>
-    <col min="6909" max="6909" width="13.81640625" style="3" customWidth="1"/>
-    <col min="6910" max="6910" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6911" max="7146" width="8.7265625" style="3"/>
-    <col min="7147" max="7148" width="18.54296875" style="3" customWidth="1"/>
-    <col min="7149" max="7164" width="8.7265625" style="3"/>
-    <col min="7165" max="7165" width="13.81640625" style="3" customWidth="1"/>
-    <col min="7166" max="7166" width="16.81640625" style="3" customWidth="1"/>
-    <col min="7167" max="7402" width="8.7265625" style="3"/>
-    <col min="7403" max="7404" width="18.54296875" style="3" customWidth="1"/>
-    <col min="7405" max="7420" width="8.7265625" style="3"/>
-    <col min="7421" max="7421" width="13.81640625" style="3" customWidth="1"/>
-    <col min="7422" max="7422" width="16.81640625" style="3" customWidth="1"/>
-    <col min="7423" max="7658" width="8.7265625" style="3"/>
-    <col min="7659" max="7660" width="18.54296875" style="3" customWidth="1"/>
-    <col min="7661" max="7676" width="8.7265625" style="3"/>
-    <col min="7677" max="7677" width="13.81640625" style="3" customWidth="1"/>
-    <col min="7678" max="7678" width="16.81640625" style="3" customWidth="1"/>
-    <col min="7679" max="7914" width="8.7265625" style="3"/>
-    <col min="7915" max="7916" width="18.54296875" style="3" customWidth="1"/>
-    <col min="7917" max="7932" width="8.7265625" style="3"/>
-    <col min="7933" max="7933" width="13.81640625" style="3" customWidth="1"/>
-    <col min="7934" max="7934" width="16.81640625" style="3" customWidth="1"/>
-    <col min="7935" max="8170" width="8.7265625" style="3"/>
-    <col min="8171" max="8172" width="18.54296875" style="3" customWidth="1"/>
-    <col min="8173" max="8188" width="8.7265625" style="3"/>
-    <col min="8189" max="8189" width="13.81640625" style="3" customWidth="1"/>
-    <col min="8190" max="8190" width="16.81640625" style="3" customWidth="1"/>
-    <col min="8191" max="8426" width="8.7265625" style="3"/>
-    <col min="8427" max="8428" width="18.54296875" style="3" customWidth="1"/>
-    <col min="8429" max="8444" width="8.7265625" style="3"/>
-    <col min="8445" max="8445" width="13.81640625" style="3" customWidth="1"/>
-    <col min="8446" max="8446" width="16.81640625" style="3" customWidth="1"/>
-    <col min="8447" max="8682" width="8.7265625" style="3"/>
-    <col min="8683" max="8684" width="18.54296875" style="3" customWidth="1"/>
-    <col min="8685" max="8700" width="8.7265625" style="3"/>
-    <col min="8701" max="8701" width="13.81640625" style="3" customWidth="1"/>
-    <col min="8702" max="8702" width="16.81640625" style="3" customWidth="1"/>
-    <col min="8703" max="8938" width="8.7265625" style="3"/>
-    <col min="8939" max="8940" width="18.54296875" style="3" customWidth="1"/>
-    <col min="8941" max="8956" width="8.7265625" style="3"/>
-    <col min="8957" max="8957" width="13.81640625" style="3" customWidth="1"/>
-    <col min="8958" max="8958" width="16.81640625" style="3" customWidth="1"/>
-    <col min="8959" max="9194" width="8.7265625" style="3"/>
-    <col min="9195" max="9196" width="18.54296875" style="3" customWidth="1"/>
-    <col min="9197" max="9212" width="8.7265625" style="3"/>
-    <col min="9213" max="9213" width="13.81640625" style="3" customWidth="1"/>
-    <col min="9214" max="9214" width="16.81640625" style="3" customWidth="1"/>
-    <col min="9215" max="9450" width="8.7265625" style="3"/>
-    <col min="9451" max="9452" width="18.54296875" style="3" customWidth="1"/>
-    <col min="9453" max="9468" width="8.7265625" style="3"/>
-    <col min="9469" max="9469" width="13.81640625" style="3" customWidth="1"/>
-    <col min="9470" max="9470" width="16.81640625" style="3" customWidth="1"/>
-    <col min="9471" max="9706" width="8.7265625" style="3"/>
-    <col min="9707" max="9708" width="18.54296875" style="3" customWidth="1"/>
-    <col min="9709" max="9724" width="8.7265625" style="3"/>
-    <col min="9725" max="9725" width="13.81640625" style="3" customWidth="1"/>
-    <col min="9726" max="9726" width="16.81640625" style="3" customWidth="1"/>
-    <col min="9727" max="9962" width="8.7265625" style="3"/>
-    <col min="9963" max="9964" width="18.54296875" style="3" customWidth="1"/>
-    <col min="9965" max="9980" width="8.7265625" style="3"/>
-    <col min="9981" max="9981" width="13.81640625" style="3" customWidth="1"/>
-    <col min="9982" max="9982" width="16.81640625" style="3" customWidth="1"/>
-    <col min="9983" max="10218" width="8.7265625" style="3"/>
-    <col min="10219" max="10220" width="18.54296875" style="3" customWidth="1"/>
-    <col min="10221" max="10236" width="8.7265625" style="3"/>
-    <col min="10237" max="10237" width="13.81640625" style="3" customWidth="1"/>
-    <col min="10238" max="10238" width="16.81640625" style="3" customWidth="1"/>
-    <col min="10239" max="10474" width="8.7265625" style="3"/>
-    <col min="10475" max="10476" width="18.54296875" style="3" customWidth="1"/>
-    <col min="10477" max="10492" width="8.7265625" style="3"/>
-    <col min="10493" max="10493" width="13.81640625" style="3" customWidth="1"/>
-    <col min="10494" max="10494" width="16.81640625" style="3" customWidth="1"/>
-    <col min="10495" max="10730" width="8.7265625" style="3"/>
-    <col min="10731" max="10732" width="18.54296875" style="3" customWidth="1"/>
-    <col min="10733" max="10748" width="8.7265625" style="3"/>
-    <col min="10749" max="10749" width="13.81640625" style="3" customWidth="1"/>
-    <col min="10750" max="10750" width="16.81640625" style="3" customWidth="1"/>
-    <col min="10751" max="10986" width="8.7265625" style="3"/>
-    <col min="10987" max="10988" width="18.54296875" style="3" customWidth="1"/>
-    <col min="10989" max="11004" width="8.7265625" style="3"/>
-    <col min="11005" max="11005" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11006" max="11006" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11007" max="11242" width="8.7265625" style="3"/>
-    <col min="11243" max="11244" width="18.54296875" style="3" customWidth="1"/>
-    <col min="11245" max="11260" width="8.7265625" style="3"/>
-    <col min="11261" max="11261" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11262" max="11262" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11263" max="11498" width="8.7265625" style="3"/>
-    <col min="11499" max="11500" width="18.54296875" style="3" customWidth="1"/>
-    <col min="11501" max="11516" width="8.7265625" style="3"/>
-    <col min="11517" max="11517" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11518" max="11518" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11519" max="11754" width="8.7265625" style="3"/>
-    <col min="11755" max="11756" width="18.54296875" style="3" customWidth="1"/>
-    <col min="11757" max="11772" width="8.7265625" style="3"/>
-    <col min="11773" max="11773" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11774" max="11774" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11775" max="12010" width="8.7265625" style="3"/>
-    <col min="12011" max="12012" width="18.54296875" style="3" customWidth="1"/>
-    <col min="12013" max="12028" width="8.7265625" style="3"/>
-    <col min="12029" max="12029" width="13.81640625" style="3" customWidth="1"/>
-    <col min="12030" max="12030" width="16.81640625" style="3" customWidth="1"/>
-    <col min="12031" max="12266" width="8.7265625" style="3"/>
-    <col min="12267" max="12268" width="18.54296875" style="3" customWidth="1"/>
-    <col min="12269" max="12284" width="8.7265625" style="3"/>
-    <col min="12285" max="12285" width="13.81640625" style="3" customWidth="1"/>
-    <col min="12286" max="12286" width="16.81640625" style="3" customWidth="1"/>
-    <col min="12287" max="12522" width="8.7265625" style="3"/>
-    <col min="12523" max="12524" width="18.54296875" style="3" customWidth="1"/>
-    <col min="12525" max="12540" width="8.7265625" style="3"/>
-    <col min="12541" max="12541" width="13.81640625" style="3" customWidth="1"/>
-    <col min="12542" max="12542" width="16.81640625" style="3" customWidth="1"/>
-    <col min="12543" max="12778" width="8.7265625" style="3"/>
-    <col min="12779" max="12780" width="18.54296875" style="3" customWidth="1"/>
-    <col min="12781" max="12796" width="8.7265625" style="3"/>
-    <col min="12797" max="12797" width="13.81640625" style="3" customWidth="1"/>
-    <col min="12798" max="12798" width="16.81640625" style="3" customWidth="1"/>
-    <col min="12799" max="13034" width="8.7265625" style="3"/>
-    <col min="13035" max="13036" width="18.54296875" style="3" customWidth="1"/>
-    <col min="13037" max="13052" width="8.7265625" style="3"/>
-    <col min="13053" max="13053" width="13.81640625" style="3" customWidth="1"/>
-    <col min="13054" max="13054" width="16.81640625" style="3" customWidth="1"/>
-    <col min="13055" max="13290" width="8.7265625" style="3"/>
-    <col min="13291" max="13292" width="18.54296875" style="3" customWidth="1"/>
-    <col min="13293" max="13308" width="8.7265625" style="3"/>
-    <col min="13309" max="13309" width="13.81640625" style="3" customWidth="1"/>
-    <col min="13310" max="13310" width="16.81640625" style="3" customWidth="1"/>
-    <col min="13311" max="13546" width="8.7265625" style="3"/>
-    <col min="13547" max="13548" width="18.54296875" style="3" customWidth="1"/>
-    <col min="13549" max="13564" width="8.7265625" style="3"/>
-    <col min="13565" max="13565" width="13.81640625" style="3" customWidth="1"/>
-    <col min="13566" max="13566" width="16.81640625" style="3" customWidth="1"/>
-    <col min="13567" max="13802" width="8.7265625" style="3"/>
-    <col min="13803" max="13804" width="18.54296875" style="3" customWidth="1"/>
-    <col min="13805" max="13820" width="8.7265625" style="3"/>
-    <col min="13821" max="13821" width="13.81640625" style="3" customWidth="1"/>
-    <col min="13822" max="13822" width="16.81640625" style="3" customWidth="1"/>
-    <col min="13823" max="14058" width="8.7265625" style="3"/>
-    <col min="14059" max="14060" width="18.54296875" style="3" customWidth="1"/>
-    <col min="14061" max="14076" width="8.7265625" style="3"/>
-    <col min="14077" max="14077" width="13.81640625" style="3" customWidth="1"/>
-    <col min="14078" max="14078" width="16.81640625" style="3" customWidth="1"/>
-    <col min="14079" max="14314" width="8.7265625" style="3"/>
-    <col min="14315" max="14316" width="18.54296875" style="3" customWidth="1"/>
-    <col min="14317" max="14332" width="8.7265625" style="3"/>
-    <col min="14333" max="14333" width="13.81640625" style="3" customWidth="1"/>
-    <col min="14334" max="14334" width="16.81640625" style="3" customWidth="1"/>
-    <col min="14335" max="14570" width="8.7265625" style="3"/>
-    <col min="14571" max="14572" width="18.54296875" style="3" customWidth="1"/>
-    <col min="14573" max="14588" width="8.7265625" style="3"/>
-    <col min="14589" max="14589" width="13.81640625" style="3" customWidth="1"/>
-    <col min="14590" max="14590" width="16.81640625" style="3" customWidth="1"/>
-    <col min="14591" max="14826" width="8.7265625" style="3"/>
-    <col min="14827" max="14828" width="18.54296875" style="3" customWidth="1"/>
-    <col min="14829" max="14844" width="8.7265625" style="3"/>
-    <col min="14845" max="14845" width="13.81640625" style="3" customWidth="1"/>
-    <col min="14846" max="14846" width="16.81640625" style="3" customWidth="1"/>
-    <col min="14847" max="15082" width="8.7265625" style="3"/>
-    <col min="15083" max="15084" width="18.54296875" style="3" customWidth="1"/>
-    <col min="15085" max="15100" width="8.7265625" style="3"/>
-    <col min="15101" max="15101" width="13.81640625" style="3" customWidth="1"/>
-    <col min="15102" max="15102" width="16.81640625" style="3" customWidth="1"/>
-    <col min="15103" max="15338" width="8.7265625" style="3"/>
-    <col min="15339" max="15340" width="18.54296875" style="3" customWidth="1"/>
-    <col min="15341" max="15356" width="8.7265625" style="3"/>
-    <col min="15357" max="15357" width="13.81640625" style="3" customWidth="1"/>
-    <col min="15358" max="15358" width="16.81640625" style="3" customWidth="1"/>
-    <col min="15359" max="15594" width="8.7265625" style="3"/>
-    <col min="15595" max="15596" width="18.54296875" style="3" customWidth="1"/>
-    <col min="15597" max="15612" width="8.7265625" style="3"/>
-    <col min="15613" max="15613" width="13.81640625" style="3" customWidth="1"/>
-    <col min="15614" max="15614" width="16.81640625" style="3" customWidth="1"/>
-    <col min="15615" max="15850" width="8.7265625" style="3"/>
-    <col min="15851" max="15852" width="18.54296875" style="3" customWidth="1"/>
-    <col min="15853" max="15868" width="8.7265625" style="3"/>
-    <col min="15869" max="15869" width="13.81640625" style="3" customWidth="1"/>
-    <col min="15870" max="15870" width="16.81640625" style="3" customWidth="1"/>
-    <col min="15871" max="16106" width="8.7265625" style="3"/>
-    <col min="16107" max="16108" width="18.54296875" style="3" customWidth="1"/>
-    <col min="16109" max="16124" width="8.7265625" style="3"/>
-    <col min="16125" max="16125" width="13.81640625" style="3" customWidth="1"/>
-    <col min="16126" max="16126" width="16.81640625" style="3" customWidth="1"/>
-    <col min="16127" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="35.26171875" style="3" customWidth="1"/>
+    <col min="2" max="19" width="10.734375" style="3" customWidth="1"/>
+    <col min="20" max="21" width="10.734375" style="4" customWidth="1"/>
+    <col min="22" max="23" width="10.734375" style="3" customWidth="1"/>
+    <col min="24" max="30" width="8.734375" style="3"/>
+    <col min="31" max="31" width="12.734375" style="3" customWidth="1"/>
+    <col min="32" max="234" width="8.734375" style="3"/>
+    <col min="235" max="236" width="18.5234375" style="3" customWidth="1"/>
+    <col min="237" max="252" width="8.734375" style="3"/>
+    <col min="253" max="253" width="13.7890625" style="3" customWidth="1"/>
+    <col min="254" max="254" width="16.7890625" style="3" customWidth="1"/>
+    <col min="255" max="490" width="8.734375" style="3"/>
+    <col min="491" max="492" width="18.5234375" style="3" customWidth="1"/>
+    <col min="493" max="508" width="8.734375" style="3"/>
+    <col min="509" max="509" width="13.7890625" style="3" customWidth="1"/>
+    <col min="510" max="510" width="16.7890625" style="3" customWidth="1"/>
+    <col min="511" max="746" width="8.734375" style="3"/>
+    <col min="747" max="748" width="18.5234375" style="3" customWidth="1"/>
+    <col min="749" max="764" width="8.734375" style="3"/>
+    <col min="765" max="765" width="13.7890625" style="3" customWidth="1"/>
+    <col min="766" max="766" width="16.7890625" style="3" customWidth="1"/>
+    <col min="767" max="1002" width="8.734375" style="3"/>
+    <col min="1003" max="1004" width="18.5234375" style="3" customWidth="1"/>
+    <col min="1005" max="1020" width="8.734375" style="3"/>
+    <col min="1021" max="1021" width="13.7890625" style="3" customWidth="1"/>
+    <col min="1022" max="1022" width="16.7890625" style="3" customWidth="1"/>
+    <col min="1023" max="1258" width="8.734375" style="3"/>
+    <col min="1259" max="1260" width="18.5234375" style="3" customWidth="1"/>
+    <col min="1261" max="1276" width="8.734375" style="3"/>
+    <col min="1277" max="1277" width="13.7890625" style="3" customWidth="1"/>
+    <col min="1278" max="1278" width="16.7890625" style="3" customWidth="1"/>
+    <col min="1279" max="1514" width="8.734375" style="3"/>
+    <col min="1515" max="1516" width="18.5234375" style="3" customWidth="1"/>
+    <col min="1517" max="1532" width="8.734375" style="3"/>
+    <col min="1533" max="1533" width="13.7890625" style="3" customWidth="1"/>
+    <col min="1534" max="1534" width="16.7890625" style="3" customWidth="1"/>
+    <col min="1535" max="1770" width="8.734375" style="3"/>
+    <col min="1771" max="1772" width="18.5234375" style="3" customWidth="1"/>
+    <col min="1773" max="1788" width="8.734375" style="3"/>
+    <col min="1789" max="1789" width="13.7890625" style="3" customWidth="1"/>
+    <col min="1790" max="1790" width="16.7890625" style="3" customWidth="1"/>
+    <col min="1791" max="2026" width="8.734375" style="3"/>
+    <col min="2027" max="2028" width="18.5234375" style="3" customWidth="1"/>
+    <col min="2029" max="2044" width="8.734375" style="3"/>
+    <col min="2045" max="2045" width="13.7890625" style="3" customWidth="1"/>
+    <col min="2046" max="2046" width="16.7890625" style="3" customWidth="1"/>
+    <col min="2047" max="2282" width="8.734375" style="3"/>
+    <col min="2283" max="2284" width="18.5234375" style="3" customWidth="1"/>
+    <col min="2285" max="2300" width="8.734375" style="3"/>
+    <col min="2301" max="2301" width="13.7890625" style="3" customWidth="1"/>
+    <col min="2302" max="2302" width="16.7890625" style="3" customWidth="1"/>
+    <col min="2303" max="2538" width="8.734375" style="3"/>
+    <col min="2539" max="2540" width="18.5234375" style="3" customWidth="1"/>
+    <col min="2541" max="2556" width="8.734375" style="3"/>
+    <col min="2557" max="2557" width="13.7890625" style="3" customWidth="1"/>
+    <col min="2558" max="2558" width="16.7890625" style="3" customWidth="1"/>
+    <col min="2559" max="2794" width="8.734375" style="3"/>
+    <col min="2795" max="2796" width="18.5234375" style="3" customWidth="1"/>
+    <col min="2797" max="2812" width="8.734375" style="3"/>
+    <col min="2813" max="2813" width="13.7890625" style="3" customWidth="1"/>
+    <col min="2814" max="2814" width="16.7890625" style="3" customWidth="1"/>
+    <col min="2815" max="3050" width="8.734375" style="3"/>
+    <col min="3051" max="3052" width="18.5234375" style="3" customWidth="1"/>
+    <col min="3053" max="3068" width="8.734375" style="3"/>
+    <col min="3069" max="3069" width="13.7890625" style="3" customWidth="1"/>
+    <col min="3070" max="3070" width="16.7890625" style="3" customWidth="1"/>
+    <col min="3071" max="3306" width="8.734375" style="3"/>
+    <col min="3307" max="3308" width="18.5234375" style="3" customWidth="1"/>
+    <col min="3309" max="3324" width="8.734375" style="3"/>
+    <col min="3325" max="3325" width="13.7890625" style="3" customWidth="1"/>
+    <col min="3326" max="3326" width="16.7890625" style="3" customWidth="1"/>
+    <col min="3327" max="3562" width="8.734375" style="3"/>
+    <col min="3563" max="3564" width="18.5234375" style="3" customWidth="1"/>
+    <col min="3565" max="3580" width="8.734375" style="3"/>
+    <col min="3581" max="3581" width="13.7890625" style="3" customWidth="1"/>
+    <col min="3582" max="3582" width="16.7890625" style="3" customWidth="1"/>
+    <col min="3583" max="3818" width="8.734375" style="3"/>
+    <col min="3819" max="3820" width="18.5234375" style="3" customWidth="1"/>
+    <col min="3821" max="3836" width="8.734375" style="3"/>
+    <col min="3837" max="3837" width="13.7890625" style="3" customWidth="1"/>
+    <col min="3838" max="3838" width="16.7890625" style="3" customWidth="1"/>
+    <col min="3839" max="4074" width="8.734375" style="3"/>
+    <col min="4075" max="4076" width="18.5234375" style="3" customWidth="1"/>
+    <col min="4077" max="4092" width="8.734375" style="3"/>
+    <col min="4093" max="4093" width="13.7890625" style="3" customWidth="1"/>
+    <col min="4094" max="4094" width="16.7890625" style="3" customWidth="1"/>
+    <col min="4095" max="4330" width="8.734375" style="3"/>
+    <col min="4331" max="4332" width="18.5234375" style="3" customWidth="1"/>
+    <col min="4333" max="4348" width="8.734375" style="3"/>
+    <col min="4349" max="4349" width="13.7890625" style="3" customWidth="1"/>
+    <col min="4350" max="4350" width="16.7890625" style="3" customWidth="1"/>
+    <col min="4351" max="4586" width="8.734375" style="3"/>
+    <col min="4587" max="4588" width="18.5234375" style="3" customWidth="1"/>
+    <col min="4589" max="4604" width="8.734375" style="3"/>
+    <col min="4605" max="4605" width="13.7890625" style="3" customWidth="1"/>
+    <col min="4606" max="4606" width="16.7890625" style="3" customWidth="1"/>
+    <col min="4607" max="4842" width="8.734375" style="3"/>
+    <col min="4843" max="4844" width="18.5234375" style="3" customWidth="1"/>
+    <col min="4845" max="4860" width="8.734375" style="3"/>
+    <col min="4861" max="4861" width="13.7890625" style="3" customWidth="1"/>
+    <col min="4862" max="4862" width="16.7890625" style="3" customWidth="1"/>
+    <col min="4863" max="5098" width="8.734375" style="3"/>
+    <col min="5099" max="5100" width="18.5234375" style="3" customWidth="1"/>
+    <col min="5101" max="5116" width="8.734375" style="3"/>
+    <col min="5117" max="5117" width="13.7890625" style="3" customWidth="1"/>
+    <col min="5118" max="5118" width="16.7890625" style="3" customWidth="1"/>
+    <col min="5119" max="5354" width="8.734375" style="3"/>
+    <col min="5355" max="5356" width="18.5234375" style="3" customWidth="1"/>
+    <col min="5357" max="5372" width="8.734375" style="3"/>
+    <col min="5373" max="5373" width="13.7890625" style="3" customWidth="1"/>
+    <col min="5374" max="5374" width="16.7890625" style="3" customWidth="1"/>
+    <col min="5375" max="5610" width="8.734375" style="3"/>
+    <col min="5611" max="5612" width="18.5234375" style="3" customWidth="1"/>
+    <col min="5613" max="5628" width="8.734375" style="3"/>
+    <col min="5629" max="5629" width="13.7890625" style="3" customWidth="1"/>
+    <col min="5630" max="5630" width="16.7890625" style="3" customWidth="1"/>
+    <col min="5631" max="5866" width="8.734375" style="3"/>
+    <col min="5867" max="5868" width="18.5234375" style="3" customWidth="1"/>
+    <col min="5869" max="5884" width="8.734375" style="3"/>
+    <col min="5885" max="5885" width="13.7890625" style="3" customWidth="1"/>
+    <col min="5886" max="5886" width="16.7890625" style="3" customWidth="1"/>
+    <col min="5887" max="6122" width="8.734375" style="3"/>
+    <col min="6123" max="6124" width="18.5234375" style="3" customWidth="1"/>
+    <col min="6125" max="6140" width="8.734375" style="3"/>
+    <col min="6141" max="6141" width="13.7890625" style="3" customWidth="1"/>
+    <col min="6142" max="6142" width="16.7890625" style="3" customWidth="1"/>
+    <col min="6143" max="6378" width="8.734375" style="3"/>
+    <col min="6379" max="6380" width="18.5234375" style="3" customWidth="1"/>
+    <col min="6381" max="6396" width="8.734375" style="3"/>
+    <col min="6397" max="6397" width="13.7890625" style="3" customWidth="1"/>
+    <col min="6398" max="6398" width="16.7890625" style="3" customWidth="1"/>
+    <col min="6399" max="6634" width="8.734375" style="3"/>
+    <col min="6635" max="6636" width="18.5234375" style="3" customWidth="1"/>
+    <col min="6637" max="6652" width="8.734375" style="3"/>
+    <col min="6653" max="6653" width="13.7890625" style="3" customWidth="1"/>
+    <col min="6654" max="6654" width="16.7890625" style="3" customWidth="1"/>
+    <col min="6655" max="6890" width="8.734375" style="3"/>
+    <col min="6891" max="6892" width="18.5234375" style="3" customWidth="1"/>
+    <col min="6893" max="6908" width="8.734375" style="3"/>
+    <col min="6909" max="6909" width="13.7890625" style="3" customWidth="1"/>
+    <col min="6910" max="6910" width="16.7890625" style="3" customWidth="1"/>
+    <col min="6911" max="7146" width="8.734375" style="3"/>
+    <col min="7147" max="7148" width="18.5234375" style="3" customWidth="1"/>
+    <col min="7149" max="7164" width="8.734375" style="3"/>
+    <col min="7165" max="7165" width="13.7890625" style="3" customWidth="1"/>
+    <col min="7166" max="7166" width="16.7890625" style="3" customWidth="1"/>
+    <col min="7167" max="7402" width="8.734375" style="3"/>
+    <col min="7403" max="7404" width="18.5234375" style="3" customWidth="1"/>
+    <col min="7405" max="7420" width="8.734375" style="3"/>
+    <col min="7421" max="7421" width="13.7890625" style="3" customWidth="1"/>
+    <col min="7422" max="7422" width="16.7890625" style="3" customWidth="1"/>
+    <col min="7423" max="7658" width="8.734375" style="3"/>
+    <col min="7659" max="7660" width="18.5234375" style="3" customWidth="1"/>
+    <col min="7661" max="7676" width="8.734375" style="3"/>
+    <col min="7677" max="7677" width="13.7890625" style="3" customWidth="1"/>
+    <col min="7678" max="7678" width="16.7890625" style="3" customWidth="1"/>
+    <col min="7679" max="7914" width="8.734375" style="3"/>
+    <col min="7915" max="7916" width="18.5234375" style="3" customWidth="1"/>
+    <col min="7917" max="7932" width="8.734375" style="3"/>
+    <col min="7933" max="7933" width="13.7890625" style="3" customWidth="1"/>
+    <col min="7934" max="7934" width="16.7890625" style="3" customWidth="1"/>
+    <col min="7935" max="8170" width="8.734375" style="3"/>
+    <col min="8171" max="8172" width="18.5234375" style="3" customWidth="1"/>
+    <col min="8173" max="8188" width="8.734375" style="3"/>
+    <col min="8189" max="8189" width="13.7890625" style="3" customWidth="1"/>
+    <col min="8190" max="8190" width="16.7890625" style="3" customWidth="1"/>
+    <col min="8191" max="8426" width="8.734375" style="3"/>
+    <col min="8427" max="8428" width="18.5234375" style="3" customWidth="1"/>
+    <col min="8429" max="8444" width="8.734375" style="3"/>
+    <col min="8445" max="8445" width="13.7890625" style="3" customWidth="1"/>
+    <col min="8446" max="8446" width="16.7890625" style="3" customWidth="1"/>
+    <col min="8447" max="8682" width="8.734375" style="3"/>
+    <col min="8683" max="8684" width="18.5234375" style="3" customWidth="1"/>
+    <col min="8685" max="8700" width="8.734375" style="3"/>
+    <col min="8701" max="8701" width="13.7890625" style="3" customWidth="1"/>
+    <col min="8702" max="8702" width="16.7890625" style="3" customWidth="1"/>
+    <col min="8703" max="8938" width="8.734375" style="3"/>
+    <col min="8939" max="8940" width="18.5234375" style="3" customWidth="1"/>
+    <col min="8941" max="8956" width="8.734375" style="3"/>
+    <col min="8957" max="8957" width="13.7890625" style="3" customWidth="1"/>
+    <col min="8958" max="8958" width="16.7890625" style="3" customWidth="1"/>
+    <col min="8959" max="9194" width="8.734375" style="3"/>
+    <col min="9195" max="9196" width="18.5234375" style="3" customWidth="1"/>
+    <col min="9197" max="9212" width="8.734375" style="3"/>
+    <col min="9213" max="9213" width="13.7890625" style="3" customWidth="1"/>
+    <col min="9214" max="9214" width="16.7890625" style="3" customWidth="1"/>
+    <col min="9215" max="9450" width="8.734375" style="3"/>
+    <col min="9451" max="9452" width="18.5234375" style="3" customWidth="1"/>
+    <col min="9453" max="9468" width="8.734375" style="3"/>
+    <col min="9469" max="9469" width="13.7890625" style="3" customWidth="1"/>
+    <col min="9470" max="9470" width="16.7890625" style="3" customWidth="1"/>
+    <col min="9471" max="9706" width="8.734375" style="3"/>
+    <col min="9707" max="9708" width="18.5234375" style="3" customWidth="1"/>
+    <col min="9709" max="9724" width="8.734375" style="3"/>
+    <col min="9725" max="9725" width="13.7890625" style="3" customWidth="1"/>
+    <col min="9726" max="9726" width="16.7890625" style="3" customWidth="1"/>
+    <col min="9727" max="9962" width="8.734375" style="3"/>
+    <col min="9963" max="9964" width="18.5234375" style="3" customWidth="1"/>
+    <col min="9965" max="9980" width="8.734375" style="3"/>
+    <col min="9981" max="9981" width="13.7890625" style="3" customWidth="1"/>
+    <col min="9982" max="9982" width="16.7890625" style="3" customWidth="1"/>
+    <col min="9983" max="10218" width="8.734375" style="3"/>
+    <col min="10219" max="10220" width="18.5234375" style="3" customWidth="1"/>
+    <col min="10221" max="10236" width="8.734375" style="3"/>
+    <col min="10237" max="10237" width="13.7890625" style="3" customWidth="1"/>
+    <col min="10238" max="10238" width="16.7890625" style="3" customWidth="1"/>
+    <col min="10239" max="10474" width="8.734375" style="3"/>
+    <col min="10475" max="10476" width="18.5234375" style="3" customWidth="1"/>
+    <col min="10477" max="10492" width="8.734375" style="3"/>
+    <col min="10493" max="10493" width="13.7890625" style="3" customWidth="1"/>
+    <col min="10494" max="10494" width="16.7890625" style="3" customWidth="1"/>
+    <col min="10495" max="10730" width="8.734375" style="3"/>
+    <col min="10731" max="10732" width="18.5234375" style="3" customWidth="1"/>
+    <col min="10733" max="10748" width="8.734375" style="3"/>
+    <col min="10749" max="10749" width="13.7890625" style="3" customWidth="1"/>
+    <col min="10750" max="10750" width="16.7890625" style="3" customWidth="1"/>
+    <col min="10751" max="10986" width="8.734375" style="3"/>
+    <col min="10987" max="10988" width="18.5234375" style="3" customWidth="1"/>
+    <col min="10989" max="11004" width="8.734375" style="3"/>
+    <col min="11005" max="11005" width="13.7890625" style="3" customWidth="1"/>
+    <col min="11006" max="11006" width="16.7890625" style="3" customWidth="1"/>
+    <col min="11007" max="11242" width="8.734375" style="3"/>
+    <col min="11243" max="11244" width="18.5234375" style="3" customWidth="1"/>
+    <col min="11245" max="11260" width="8.734375" style="3"/>
+    <col min="11261" max="11261" width="13.7890625" style="3" customWidth="1"/>
+    <col min="11262" max="11262" width="16.7890625" style="3" customWidth="1"/>
+    <col min="11263" max="11498" width="8.734375" style="3"/>
+    <col min="11499" max="11500" width="18.5234375" style="3" customWidth="1"/>
+    <col min="11501" max="11516" width="8.734375" style="3"/>
+    <col min="11517" max="11517" width="13.7890625" style="3" customWidth="1"/>
+    <col min="11518" max="11518" width="16.7890625" style="3" customWidth="1"/>
+    <col min="11519" max="11754" width="8.734375" style="3"/>
+    <col min="11755" max="11756" width="18.5234375" style="3" customWidth="1"/>
+    <col min="11757" max="11772" width="8.734375" style="3"/>
+    <col min="11773" max="11773" width="13.7890625" style="3" customWidth="1"/>
+    <col min="11774" max="11774" width="16.7890625" style="3" customWidth="1"/>
+    <col min="11775" max="12010" width="8.734375" style="3"/>
+    <col min="12011" max="12012" width="18.5234375" style="3" customWidth="1"/>
+    <col min="12013" max="12028" width="8.734375" style="3"/>
+    <col min="12029" max="12029" width="13.7890625" style="3" customWidth="1"/>
+    <col min="12030" max="12030" width="16.7890625" style="3" customWidth="1"/>
+    <col min="12031" max="12266" width="8.734375" style="3"/>
+    <col min="12267" max="12268" width="18.5234375" style="3" customWidth="1"/>
+    <col min="12269" max="12284" width="8.734375" style="3"/>
+    <col min="12285" max="12285" width="13.7890625" style="3" customWidth="1"/>
+    <col min="12286" max="12286" width="16.7890625" style="3" customWidth="1"/>
+    <col min="12287" max="12522" width="8.734375" style="3"/>
+    <col min="12523" max="12524" width="18.5234375" style="3" customWidth="1"/>
+    <col min="12525" max="12540" width="8.734375" style="3"/>
+    <col min="12541" max="12541" width="13.7890625" style="3" customWidth="1"/>
+    <col min="12542" max="12542" width="16.7890625" style="3" customWidth="1"/>
+    <col min="12543" max="12778" width="8.734375" style="3"/>
+    <col min="12779" max="12780" width="18.5234375" style="3" customWidth="1"/>
+    <col min="12781" max="12796" width="8.734375" style="3"/>
+    <col min="12797" max="12797" width="13.7890625" style="3" customWidth="1"/>
+    <col min="12798" max="12798" width="16.7890625" style="3" customWidth="1"/>
+    <col min="12799" max="13034" width="8.734375" style="3"/>
+    <col min="13035" max="13036" width="18.5234375" style="3" customWidth="1"/>
+    <col min="13037" max="13052" width="8.734375" style="3"/>
+    <col min="13053" max="13053" width="13.7890625" style="3" customWidth="1"/>
+    <col min="13054" max="13054" width="16.7890625" style="3" customWidth="1"/>
+    <col min="13055" max="13290" width="8.734375" style="3"/>
+    <col min="13291" max="13292" width="18.5234375" style="3" customWidth="1"/>
+    <col min="13293" max="13308" width="8.734375" style="3"/>
+    <col min="13309" max="13309" width="13.7890625" style="3" customWidth="1"/>
+    <col min="13310" max="13310" width="16.7890625" style="3" customWidth="1"/>
+    <col min="13311" max="13546" width="8.734375" style="3"/>
+    <col min="13547" max="13548" width="18.5234375" style="3" customWidth="1"/>
+    <col min="13549" max="13564" width="8.734375" style="3"/>
+    <col min="13565" max="13565" width="13.7890625" style="3" customWidth="1"/>
+    <col min="13566" max="13566" width="16.7890625" style="3" customWidth="1"/>
+    <col min="13567" max="13802" width="8.734375" style="3"/>
+    <col min="13803" max="13804" width="18.5234375" style="3" customWidth="1"/>
+    <col min="13805" max="13820" width="8.734375" style="3"/>
+    <col min="13821" max="13821" width="13.7890625" style="3" customWidth="1"/>
+    <col min="13822" max="13822" width="16.7890625" style="3" customWidth="1"/>
+    <col min="13823" max="14058" width="8.734375" style="3"/>
+    <col min="14059" max="14060" width="18.5234375" style="3" customWidth="1"/>
+    <col min="14061" max="14076" width="8.734375" style="3"/>
+    <col min="14077" max="14077" width="13.7890625" style="3" customWidth="1"/>
+    <col min="14078" max="14078" width="16.7890625" style="3" customWidth="1"/>
+    <col min="14079" max="14314" width="8.734375" style="3"/>
+    <col min="14315" max="14316" width="18.5234375" style="3" customWidth="1"/>
+    <col min="14317" max="14332" width="8.734375" style="3"/>
+    <col min="14333" max="14333" width="13.7890625" style="3" customWidth="1"/>
+    <col min="14334" max="14334" width="16.7890625" style="3" customWidth="1"/>
+    <col min="14335" max="14570" width="8.734375" style="3"/>
+    <col min="14571" max="14572" width="18.5234375" style="3" customWidth="1"/>
+    <col min="14573" max="14588" width="8.734375" style="3"/>
+    <col min="14589" max="14589" width="13.7890625" style="3" customWidth="1"/>
+    <col min="14590" max="14590" width="16.7890625" style="3" customWidth="1"/>
+    <col min="14591" max="14826" width="8.734375" style="3"/>
+    <col min="14827" max="14828" width="18.5234375" style="3" customWidth="1"/>
+    <col min="14829" max="14844" width="8.734375" style="3"/>
+    <col min="14845" max="14845" width="13.7890625" style="3" customWidth="1"/>
+    <col min="14846" max="14846" width="16.7890625" style="3" customWidth="1"/>
+    <col min="14847" max="15082" width="8.734375" style="3"/>
+    <col min="15083" max="15084" width="18.5234375" style="3" customWidth="1"/>
+    <col min="15085" max="15100" width="8.734375" style="3"/>
+    <col min="15101" max="15101" width="13.7890625" style="3" customWidth="1"/>
+    <col min="15102" max="15102" width="16.7890625" style="3" customWidth="1"/>
+    <col min="15103" max="15338" width="8.734375" style="3"/>
+    <col min="15339" max="15340" width="18.5234375" style="3" customWidth="1"/>
+    <col min="15341" max="15356" width="8.734375" style="3"/>
+    <col min="15357" max="15357" width="13.7890625" style="3" customWidth="1"/>
+    <col min="15358" max="15358" width="16.7890625" style="3" customWidth="1"/>
+    <col min="15359" max="15594" width="8.734375" style="3"/>
+    <col min="15595" max="15596" width="18.5234375" style="3" customWidth="1"/>
+    <col min="15597" max="15612" width="8.734375" style="3"/>
+    <col min="15613" max="15613" width="13.7890625" style="3" customWidth="1"/>
+    <col min="15614" max="15614" width="16.7890625" style="3" customWidth="1"/>
+    <col min="15615" max="15850" width="8.734375" style="3"/>
+    <col min="15851" max="15852" width="18.5234375" style="3" customWidth="1"/>
+    <col min="15853" max="15868" width="8.734375" style="3"/>
+    <col min="15869" max="15869" width="13.7890625" style="3" customWidth="1"/>
+    <col min="15870" max="15870" width="16.7890625" style="3" customWidth="1"/>
+    <col min="15871" max="16106" width="8.734375" style="3"/>
+    <col min="16107" max="16108" width="18.5234375" style="3" customWidth="1"/>
+    <col min="16109" max="16124" width="8.734375" style="3"/>
+    <col min="16125" max="16125" width="13.7890625" style="3" customWidth="1"/>
+    <col min="16126" max="16126" width="16.7890625" style="3" customWidth="1"/>
+    <col min="16127" max="16384" width="8.734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="23" spans="1:55" s="1" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:55" s="1" customFormat="1" ht="135.30000000000001" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -10459,7 +10459,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:55" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:55" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -10546,7 +10546,7 @@
       <c r="AW24" s="7"/>
       <c r="AX24" s="7"/>
     </row>
-    <row r="25" spans="1:55" s="1" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:55" s="1" customFormat="1" ht="49.2" x14ac:dyDescent="0.4">
       <c r="C25" s="1" t="s">
         <v>30</v>
       </c>
@@ -10573,7 +10573,7 @@
       </c>
       <c r="AN25" s="21"/>
     </row>
-    <row r="26" spans="1:55" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:55" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="9">
         <v>42759</v>
       </c>
@@ -10638,7 +10638,7 @@
       <c r="BB26" s="7"/>
       <c r="BC26" s="7"/>
     </row>
-    <row r="27" spans="1:55" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:55" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="9">
         <v>42759</v>
       </c>
@@ -10703,7 +10703,7 @@
       <c r="BB27" s="7"/>
       <c r="BC27" s="7"/>
     </row>
-    <row r="28" spans="1:55" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:55" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="9">
         <v>42767</v>
       </c>
@@ -10768,7 +10768,7 @@
       <c r="BB28" s="7"/>
       <c r="BC28" s="7"/>
     </row>
-    <row r="29" spans="1:55" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:55" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="9">
         <v>42864</v>
       </c>
@@ -10833,7 +10833,7 @@
       <c r="BB29" s="7"/>
       <c r="BC29" s="7"/>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.4">
       <c r="B30" s="9">
         <v>43046</v>
       </c>
@@ -10898,7 +10898,7 @@
       <c r="BB30" s="7"/>
       <c r="BC30" s="7"/>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.4">
       <c r="B31" s="9">
         <v>43151</v>
       </c>
@@ -10963,7 +10963,7 @@
       <c r="BB31" s="7"/>
       <c r="BC31" s="7"/>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>64</v>
       </c>
@@ -11097,7 +11097,7 @@
       </c>
       <c r="BC32" s="7"/>
     </row>
-    <row r="33" spans="1:55" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:55" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -11222,7 +11222,7 @@
       </c>
       <c r="BC33" s="7"/>
     </row>
-    <row r="34" spans="1:55" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:55" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -11347,7 +11347,7 @@
       </c>
       <c r="BC34" s="7"/>
     </row>
-    <row r="35" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
@@ -11482,7 +11482,7 @@
       </c>
       <c r="BC35" s="7"/>
     </row>
-    <row r="36" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -11617,7 +11617,7 @@
       </c>
       <c r="BC36" s="7"/>
     </row>
-    <row r="37" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>67</v>
       </c>
@@ -11752,7 +11752,7 @@
       </c>
       <c r="BC37" s="7"/>
     </row>
-    <row r="38" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>68</v>
       </c>
@@ -11887,7 +11887,7 @@
       </c>
       <c r="BC38" s="7"/>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>69</v>
       </c>
@@ -12022,7 +12022,7 @@
       </c>
       <c r="BC39" s="7"/>
     </row>
-    <row r="40" spans="1:55" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:55" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -12161,7 +12161,7 @@
       </c>
       <c r="BC40" s="7"/>
     </row>
-    <row r="41" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AN41" s="8"/>
       <c r="AT41" s="6"/>
       <c r="AU41" s="6"/>
@@ -12174,7 +12174,7 @@
       <c r="BB41" s="7"/>
       <c r="BC41" s="7"/>
     </row>
-    <row r="42" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AN42" s="8"/>
       <c r="AT42" s="6"/>
       <c r="AU42" s="6"/>
@@ -12187,7 +12187,7 @@
       <c r="BB42" s="7"/>
       <c r="BC42" s="7"/>
     </row>
-    <row r="43" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AN43" s="8"/>
       <c r="AT43" s="6"/>
       <c r="AU43" s="6"/>
@@ -12200,7 +12200,7 @@
       <c r="BB43" s="7"/>
       <c r="BC43" s="7"/>
     </row>
-    <row r="44" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AN44" s="8"/>
       <c r="AT44" s="6"/>
       <c r="AU44" s="6"/>
@@ -12213,7 +12213,7 @@
       <c r="BB44" s="7"/>
       <c r="BC44" s="7"/>
     </row>
-    <row r="45" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AN45" s="8"/>
       <c r="AT45" s="6"/>
       <c r="AU45" s="6"/>
@@ -12226,7 +12226,7 @@
       <c r="BB45" s="7"/>
       <c r="BC45" s="7"/>
     </row>
-    <row r="46" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AT46" s="6"/>
       <c r="AU46" s="6"/>
       <c r="AV46" s="6"/>
@@ -12238,7 +12238,7 @@
       <c r="BB46" s="7"/>
       <c r="BC46" s="7"/>
     </row>
-    <row r="47" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AT47" s="6"/>
       <c r="AU47" s="6"/>
       <c r="AV47" s="6"/>
@@ -12250,7 +12250,7 @@
       <c r="BB47" s="7"/>
       <c r="BC47" s="7"/>
     </row>
-    <row r="48" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AT48" s="6"/>
       <c r="AU48" s="6"/>
       <c r="AV48" s="6"/>
@@ -12262,7 +12262,7 @@
       <c r="BB48" s="7"/>
       <c r="BC48" s="7"/>
     </row>
-    <row r="49" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AT49" s="6"/>
       <c r="AU49" s="6"/>
       <c r="AV49" s="6"/>
@@ -12274,13 +12274,13 @@
       <c r="BB49" s="7"/>
       <c r="BC49" s="7"/>
     </row>
-    <row r="50" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AT50" s="6"/>
       <c r="AU50" s="6"/>
       <c r="AV50" s="6"/>
       <c r="AW50" s="6"/>
     </row>
-    <row r="51" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>49</v>
       </c>
@@ -12306,7 +12306,7 @@
         <v>1.3544622498376095</v>
       </c>
     </row>
-    <row r="52" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>50</v>
       </c>
@@ -12331,7 +12331,7 @@
         <v>7.3200521182799003E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AD53" s="11"/>
       <c r="AE53" s="7" t="s">
         <v>36</v>
@@ -12349,7 +12349,7 @@
         <v>5.40439729431922</v>
       </c>
     </row>
-    <row r="54" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AD54" s="11" t="s">
         <v>39</v>
       </c>
@@ -12369,7 +12369,7 @@
         <v>1.2080612074720116</v>
       </c>
     </row>
-    <row r="55" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AD55" s="12"/>
       <c r="AE55" s="7" t="s">
         <v>41</v>
@@ -12387,7 +12387,7 @@
         <v>1.5008632922032075</v>
       </c>
     </row>
-    <row r="56" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AD56" s="11" t="s">
         <v>42</v>
       </c>
@@ -12407,7 +12407,7 @@
         <v>1.1348606862892126</v>
       </c>
     </row>
-    <row r="57" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AD57" s="10"/>
       <c r="AE57" s="7" t="s">
         <v>44</v>
@@ -12425,7 +12425,7 @@
         <v>1.5740638133860065</v>
       </c>
     </row>
-    <row r="58" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AD58" s="11" t="s">
         <v>45</v>
       </c>
@@ -12445,7 +12445,7 @@
         <v>0.22984963651398888</v>
       </c>
     </row>
-    <row r="59" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:55" x14ac:dyDescent="0.4">
       <c r="AD59" s="11" t="s">
         <v>47</v>
       </c>

</xml_diff>